<commit_message>
Dec 9 Commit 2
</commit_message>
<xml_diff>
--- a/Ajith_KUBS_CEN_GeneralLedger12/Test-data/GLTestData.xlsx
+++ b/Ajith_KUBS_CEN_GeneralLedger12/Test-data/GLTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AllMastersTestDataInfo" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="452">
   <si>
     <t>Creation of Asset AutoMaster</t>
   </si>
@@ -1242,12 +1242,6 @@
     <t>Modified13915</t>
   </si>
   <si>
-    <t>52282</t>
-  </si>
-  <si>
-    <t>JV_AZE_JAN2024_52357</t>
-  </si>
-  <si>
     <t>52358</t>
   </si>
   <si>
@@ -1341,9 +1335,6 @@
     <t>CurrenyForGL Balances Report</t>
   </si>
   <si>
-    <t>JV_AZE_JAN2024_52968</t>
-  </si>
-  <si>
     <t>53054</t>
   </si>
   <si>
@@ -1351,6 +1342,42 @@
   </si>
   <si>
     <t xml:space="preserve"> 1120201001 - FD with Central Bank of India (Non-Current) </t>
+  </si>
+  <si>
+    <t>JobCode</t>
+  </si>
+  <si>
+    <t>JobName</t>
+  </si>
+  <si>
+    <t>ApplicationName</t>
+  </si>
+  <si>
+    <t>ModuleCode</t>
+  </si>
+  <si>
+    <t>ProcessName</t>
+  </si>
+  <si>
+    <t>JobType</t>
+  </si>
+  <si>
+    <t>NumberOfThreads</t>
+  </si>
+  <si>
+    <t>SequenceNumber</t>
+  </si>
+  <si>
+    <t>End Of Day</t>
+  </si>
+  <si>
+    <t>Process Day Change</t>
+  </si>
+  <si>
+    <t>TestJob</t>
+  </si>
+  <si>
+    <t>TestModule</t>
   </si>
 </sst>
 </file>
@@ -1899,12 +1926,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" hidden="true" width="21.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" hidden="true" width="0.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="20.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" hidden="true" width="4.140625" collapsed="true"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.28515625" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="4.140625" hidden="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2142,9 +2169,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2262,33 +2289,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="10" max="13" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="29" max="31" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="13" width="12" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="22" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="13" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="31" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="24.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="37" customFormat="1">
@@ -5605,32 +5632,32 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AV48"/>
+  <dimension ref="A1:BM48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AU32" sqref="AU32"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="AW36" sqref="AW36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7734375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.08984375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="50.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="36.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="45.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="36.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="40.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="49.140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="38.85546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="49.5703125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="44.42578125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="23.2890625" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="35" max="35" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="50.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="36.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="45.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="36.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="40.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="49.140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="38.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="49.5703125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="44.42578125" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="36.42578125" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="37.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48">
+    <row r="1" spans="1:65">
       <c r="A1" s="19" t="s">
         <v>23</v>
       </c>
@@ -5713,64 +5740,97 @@
         <v>377</v>
       </c>
       <c r="AB1" s="19" t="s">
+        <v>434</v>
+      </c>
+      <c r="AC1" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="AD1" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="AE1" s="19" t="s">
+        <v>410</v>
+      </c>
+      <c r="AF1" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="AG1" s="19" t="s">
+        <v>412</v>
+      </c>
+      <c r="AH1" s="19" t="s">
+        <v>413</v>
+      </c>
+      <c r="AI1" s="19" t="s">
+        <v>414</v>
+      </c>
+      <c r="AJ1" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="AK1" s="19" t="s">
+        <v>435</v>
+      </c>
+      <c r="AL1" s="19" t="s">
+        <v>427</v>
+      </c>
+      <c r="AM1" s="19" t="s">
+        <v>428</v>
+      </c>
+      <c r="AN1" s="19" t="s">
+        <v>429</v>
+      </c>
+      <c r="AO1" s="19" t="s">
+        <v>430</v>
+      </c>
+      <c r="AP1" s="19" t="s">
+        <v>431</v>
+      </c>
+      <c r="AQ1" s="19" t="s">
+        <v>432</v>
+      </c>
+      <c r="AR1" s="19" t="s">
+        <v>433</v>
+      </c>
+      <c r="AS1" s="19" t="s">
         <v>436</v>
       </c>
-      <c r="AC1" s="19" t="s">
-        <v>409</v>
-      </c>
-      <c r="AD1" s="19" t="s">
-        <v>411</v>
-      </c>
-      <c r="AE1" s="19" t="s">
-        <v>412</v>
-      </c>
-      <c r="AF1" s="19" t="s">
-        <v>413</v>
-      </c>
-      <c r="AG1" s="19" t="s">
-        <v>414</v>
-      </c>
-      <c r="AH1" s="19" t="s">
-        <v>415</v>
-      </c>
-      <c r="AI1" s="19" t="s">
-        <v>416</v>
-      </c>
-      <c r="AJ1" s="19" t="s">
-        <v>417</v>
-      </c>
-      <c r="AK1" s="19" t="s">
-        <v>437</v>
-      </c>
-      <c r="AL1" s="19" t="s">
-        <v>429</v>
-      </c>
-      <c r="AM1" s="19" t="s">
-        <v>430</v>
-      </c>
-      <c r="AN1" s="19" t="s">
-        <v>431</v>
-      </c>
-      <c r="AO1" s="19" t="s">
-        <v>432</v>
-      </c>
-      <c r="AP1" s="19" t="s">
-        <v>433</v>
-      </c>
-      <c r="AQ1" s="19" t="s">
-        <v>434</v>
-      </c>
-      <c r="AR1" s="19" t="s">
-        <v>435</v>
-      </c>
-      <c r="AS1" s="19" t="s">
-        <v>438</v>
-      </c>
-      <c r="AT1" s="19"/>
-      <c r="AU1" s="19"/>
-      <c r="AV1" s="19"/>
-    </row>
-    <row r="2" spans="1:48" ht="15.75">
+      <c r="AT1" s="19" t="s">
+        <v>440</v>
+      </c>
+      <c r="AU1" s="19" t="s">
+        <v>441</v>
+      </c>
+      <c r="AV1" s="19" t="s">
+        <v>442</v>
+      </c>
+      <c r="AW1" s="19" t="s">
+        <v>443</v>
+      </c>
+      <c r="AX1" s="19" t="s">
+        <v>444</v>
+      </c>
+      <c r="AY1" s="19" t="s">
+        <v>445</v>
+      </c>
+      <c r="AZ1" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="BA1" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="BB1" s="19"/>
+      <c r="BC1" s="19"/>
+      <c r="BD1" s="19"/>
+      <c r="BE1" s="19"/>
+      <c r="BF1" s="19"/>
+      <c r="BG1" s="19"/>
+      <c r="BH1" s="19"/>
+      <c r="BI1" s="19"/>
+      <c r="BJ1" s="19"/>
+      <c r="BK1" s="19"/>
+      <c r="BL1" s="19"/>
+      <c r="BM1" s="19"/>
+    </row>
+    <row r="2" spans="1:65" ht="15.75">
       <c r="A2" s="20" t="s">
         <v>248</v>
       </c>
@@ -5846,8 +5906,16 @@
       <c r="AQ2" s="35"/>
       <c r="AR2" s="35"/>
       <c r="AS2" s="35"/>
-    </row>
-    <row r="3" spans="1:48" ht="15.75">
+      <c r="AT2" s="20"/>
+      <c r="AU2" s="20"/>
+      <c r="AV2" s="20"/>
+      <c r="AW2" s="20"/>
+      <c r="AX2" s="20"/>
+      <c r="AY2" s="20"/>
+      <c r="AZ2" s="20"/>
+      <c r="BA2" s="20"/>
+    </row>
+    <row r="3" spans="1:65" ht="15.75">
       <c r="A3" s="20" t="s">
         <v>260</v>
       </c>
@@ -5903,8 +5971,16 @@
       <c r="AQ3" s="35"/>
       <c r="AR3" s="35"/>
       <c r="AS3" s="35"/>
-    </row>
-    <row r="4" spans="1:48" ht="15.75">
+      <c r="AT3" s="20"/>
+      <c r="AU3" s="20"/>
+      <c r="AV3" s="20"/>
+      <c r="AW3" s="20"/>
+      <c r="AX3" s="20"/>
+      <c r="AY3" s="20"/>
+      <c r="AZ3" s="20"/>
+      <c r="BA3" s="20"/>
+    </row>
+    <row r="4" spans="1:65" ht="15.75">
       <c r="A4" s="20" t="s">
         <v>261</v>
       </c>
@@ -5956,8 +6032,16 @@
       <c r="AQ4" s="35"/>
       <c r="AR4" s="35"/>
       <c r="AS4" s="35"/>
-    </row>
-    <row r="5" spans="1:48" ht="15.75">
+      <c r="AT4" s="20"/>
+      <c r="AU4" s="20"/>
+      <c r="AV4" s="20"/>
+      <c r="AW4" s="20"/>
+      <c r="AX4" s="20"/>
+      <c r="AY4" s="20"/>
+      <c r="AZ4" s="20"/>
+      <c r="BA4" s="20"/>
+    </row>
+    <row r="5" spans="1:65" ht="15.75">
       <c r="A5" s="20" t="s">
         <v>262</v>
       </c>
@@ -6009,8 +6093,16 @@
       <c r="AQ5" s="35"/>
       <c r="AR5" s="35"/>
       <c r="AS5" s="35"/>
-    </row>
-    <row r="6" spans="1:48" ht="15.75">
+      <c r="AT5" s="20"/>
+      <c r="AU5" s="20"/>
+      <c r="AV5" s="20"/>
+      <c r="AW5" s="20"/>
+      <c r="AX5" s="20"/>
+      <c r="AY5" s="20"/>
+      <c r="AZ5" s="20"/>
+      <c r="BA5" s="20"/>
+    </row>
+    <row r="6" spans="1:65" ht="15.75">
       <c r="A6" s="20" t="s">
         <v>266</v>
       </c>
@@ -6082,8 +6174,16 @@
       <c r="AQ6" s="35"/>
       <c r="AR6" s="35"/>
       <c r="AS6" s="35"/>
-    </row>
-    <row r="7" spans="1:48" ht="15.75">
+      <c r="AT6" s="20"/>
+      <c r="AU6" s="20"/>
+      <c r="AV6" s="20"/>
+      <c r="AW6" s="20"/>
+      <c r="AX6" s="20"/>
+      <c r="AY6" s="20"/>
+      <c r="AZ6" s="20"/>
+      <c r="BA6" s="20"/>
+    </row>
+    <row r="7" spans="1:65" ht="15.75">
       <c r="A7" s="20" t="s">
         <v>271</v>
       </c>
@@ -6139,8 +6239,16 @@
       <c r="AQ7" s="35"/>
       <c r="AR7" s="35"/>
       <c r="AS7" s="35"/>
-    </row>
-    <row r="8" spans="1:48" ht="15.75">
+      <c r="AT7" s="20"/>
+      <c r="AU7" s="20"/>
+      <c r="AV7" s="20"/>
+      <c r="AW7" s="20"/>
+      <c r="AX7" s="20"/>
+      <c r="AY7" s="20"/>
+      <c r="AZ7" s="20"/>
+      <c r="BA7" s="20"/>
+    </row>
+    <row r="8" spans="1:65" ht="15.75">
       <c r="A8" s="20" t="s">
         <v>272</v>
       </c>
@@ -6192,8 +6300,16 @@
       <c r="AQ8" s="35"/>
       <c r="AR8" s="35"/>
       <c r="AS8" s="35"/>
-    </row>
-    <row r="9" spans="1:48" ht="15.75">
+      <c r="AT8" s="20"/>
+      <c r="AU8" s="20"/>
+      <c r="AV8" s="20"/>
+      <c r="AW8" s="20"/>
+      <c r="AX8" s="20"/>
+      <c r="AY8" s="20"/>
+      <c r="AZ8" s="20"/>
+      <c r="BA8" s="20"/>
+    </row>
+    <row r="9" spans="1:65" ht="15.75">
       <c r="A9" s="20" t="s">
         <v>273</v>
       </c>
@@ -6245,8 +6361,16 @@
       <c r="AQ9" s="35"/>
       <c r="AR9" s="35"/>
       <c r="AS9" s="35"/>
-    </row>
-    <row r="10" spans="1:48" ht="15.75">
+      <c r="AT9" s="20"/>
+      <c r="AU9" s="20"/>
+      <c r="AV9" s="20"/>
+      <c r="AW9" s="20"/>
+      <c r="AX9" s="20"/>
+      <c r="AY9" s="20"/>
+      <c r="AZ9" s="20"/>
+      <c r="BA9" s="20"/>
+    </row>
+    <row r="10" spans="1:65" ht="15.75">
       <c r="A10" s="20" t="s">
         <v>274</v>
       </c>
@@ -6318,8 +6442,16 @@
       <c r="AQ10" s="35"/>
       <c r="AR10" s="35"/>
       <c r="AS10" s="35"/>
-    </row>
-    <row r="11" spans="1:48" ht="15.75">
+      <c r="AT10" s="20"/>
+      <c r="AU10" s="20"/>
+      <c r="AV10" s="20"/>
+      <c r="AW10" s="20"/>
+      <c r="AX10" s="20"/>
+      <c r="AY10" s="20"/>
+      <c r="AZ10" s="20"/>
+      <c r="BA10" s="20"/>
+    </row>
+    <row r="11" spans="1:65" ht="15.75">
       <c r="A11" s="20" t="s">
         <v>275</v>
       </c>
@@ -6375,8 +6507,16 @@
       <c r="AQ11" s="35"/>
       <c r="AR11" s="35"/>
       <c r="AS11" s="35"/>
-    </row>
-    <row r="12" spans="1:48" ht="15.75">
+      <c r="AT11" s="20"/>
+      <c r="AU11" s="20"/>
+      <c r="AV11" s="20"/>
+      <c r="AW11" s="20"/>
+      <c r="AX11" s="20"/>
+      <c r="AY11" s="20"/>
+      <c r="AZ11" s="20"/>
+      <c r="BA11" s="20"/>
+    </row>
+    <row r="12" spans="1:65" ht="15.75">
       <c r="A12" s="20" t="s">
         <v>276</v>
       </c>
@@ -6428,8 +6568,16 @@
       <c r="AQ12" s="35"/>
       <c r="AR12" s="35"/>
       <c r="AS12" s="35"/>
-    </row>
-    <row r="13" spans="1:48" ht="15.75">
+      <c r="AT12" s="20"/>
+      <c r="AU12" s="20"/>
+      <c r="AV12" s="20"/>
+      <c r="AW12" s="20"/>
+      <c r="AX12" s="20"/>
+      <c r="AY12" s="20"/>
+      <c r="AZ12" s="20"/>
+      <c r="BA12" s="20"/>
+    </row>
+    <row r="13" spans="1:65" ht="15.75">
       <c r="A13" s="20" t="s">
         <v>277</v>
       </c>
@@ -6481,8 +6629,16 @@
       <c r="AQ13" s="35"/>
       <c r="AR13" s="35"/>
       <c r="AS13" s="35"/>
-    </row>
-    <row r="14" spans="1:48" ht="15.75">
+      <c r="AT13" s="20"/>
+      <c r="AU13" s="20"/>
+      <c r="AV13" s="20"/>
+      <c r="AW13" s="20"/>
+      <c r="AX13" s="20"/>
+      <c r="AY13" s="20"/>
+      <c r="AZ13" s="20"/>
+      <c r="BA13" s="20"/>
+    </row>
+    <row r="14" spans="1:65" ht="15.75">
       <c r="A14" s="20" t="s">
         <v>286</v>
       </c>
@@ -6554,8 +6710,16 @@
       <c r="AQ14" s="35"/>
       <c r="AR14" s="35"/>
       <c r="AS14" s="35"/>
-    </row>
-    <row r="15" spans="1:48" ht="15.75">
+      <c r="AT14" s="20"/>
+      <c r="AU14" s="20"/>
+      <c r="AV14" s="20"/>
+      <c r="AW14" s="20"/>
+      <c r="AX14" s="20"/>
+      <c r="AY14" s="20"/>
+      <c r="AZ14" s="20"/>
+      <c r="BA14" s="20"/>
+    </row>
+    <row r="15" spans="1:65" ht="15.75">
       <c r="A15" s="20" t="s">
         <v>288</v>
       </c>
@@ -6611,8 +6775,16 @@
       <c r="AQ15" s="35"/>
       <c r="AR15" s="35"/>
       <c r="AS15" s="35"/>
-    </row>
-    <row r="16" spans="1:48" ht="15.75">
+      <c r="AT15" s="20"/>
+      <c r="AU15" s="20"/>
+      <c r="AV15" s="20"/>
+      <c r="AW15" s="20"/>
+      <c r="AX15" s="20"/>
+      <c r="AY15" s="20"/>
+      <c r="AZ15" s="20"/>
+      <c r="BA15" s="20"/>
+    </row>
+    <row r="16" spans="1:65" ht="15.75">
       <c r="A16" s="20" t="s">
         <v>289</v>
       </c>
@@ -6664,8 +6836,16 @@
       <c r="AQ16" s="35"/>
       <c r="AR16" s="35"/>
       <c r="AS16" s="35"/>
-    </row>
-    <row r="17" spans="1:45" ht="15.75">
+      <c r="AT16" s="20"/>
+      <c r="AU16" s="20"/>
+      <c r="AV16" s="20"/>
+      <c r="AW16" s="20"/>
+      <c r="AX16" s="20"/>
+      <c r="AY16" s="20"/>
+      <c r="AZ16" s="20"/>
+      <c r="BA16" s="20"/>
+    </row>
+    <row r="17" spans="1:53" ht="15.75">
       <c r="A17" s="20" t="s">
         <v>290</v>
       </c>
@@ -6717,8 +6897,16 @@
       <c r="AQ17" s="35"/>
       <c r="AR17" s="35"/>
       <c r="AS17" s="35"/>
-    </row>
-    <row r="18" spans="1:45" ht="15.75">
+      <c r="AT17" s="20"/>
+      <c r="AU17" s="20"/>
+      <c r="AV17" s="20"/>
+      <c r="AW17" s="20"/>
+      <c r="AX17" s="20"/>
+      <c r="AY17" s="20"/>
+      <c r="AZ17" s="20"/>
+      <c r="BA17" s="20"/>
+    </row>
+    <row r="18" spans="1:53" ht="15.75">
       <c r="A18" s="20" t="s">
         <v>294</v>
       </c>
@@ -6790,8 +6978,16 @@
       <c r="AQ18" s="35"/>
       <c r="AR18" s="35"/>
       <c r="AS18" s="35"/>
-    </row>
-    <row r="19" spans="1:45" ht="15.75">
+      <c r="AT18" s="20"/>
+      <c r="AU18" s="20"/>
+      <c r="AV18" s="20"/>
+      <c r="AW18" s="20"/>
+      <c r="AX18" s="20"/>
+      <c r="AY18" s="20"/>
+      <c r="AZ18" s="20"/>
+      <c r="BA18" s="20"/>
+    </row>
+    <row r="19" spans="1:53" ht="15.75">
       <c r="A19" s="20" t="s">
         <v>295</v>
       </c>
@@ -6799,7 +6995,7 @@
         <v>299</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D19" s="41" t="s">
         <v>239</v>
@@ -6847,8 +7043,16 @@
       <c r="AQ19" s="35"/>
       <c r="AR19" s="35"/>
       <c r="AS19" s="35"/>
-    </row>
-    <row r="20" spans="1:45" ht="15.75">
+      <c r="AT19" s="20"/>
+      <c r="AU19" s="20"/>
+      <c r="AV19" s="20"/>
+      <c r="AW19" s="20"/>
+      <c r="AX19" s="20"/>
+      <c r="AY19" s="20"/>
+      <c r="AZ19" s="20"/>
+      <c r="BA19" s="20"/>
+    </row>
+    <row r="20" spans="1:53" ht="15.75">
       <c r="A20" s="20" t="s">
         <v>296</v>
       </c>
@@ -6900,8 +7104,16 @@
       <c r="AQ20" s="35"/>
       <c r="AR20" s="35"/>
       <c r="AS20" s="35"/>
-    </row>
-    <row r="21" spans="1:45" ht="15.75">
+      <c r="AT20" s="20"/>
+      <c r="AU20" s="20"/>
+      <c r="AV20" s="20"/>
+      <c r="AW20" s="20"/>
+      <c r="AX20" s="20"/>
+      <c r="AY20" s="20"/>
+      <c r="AZ20" s="20"/>
+      <c r="BA20" s="20"/>
+    </row>
+    <row r="21" spans="1:53" ht="15.75">
       <c r="A21" s="20" t="s">
         <v>297</v>
       </c>
@@ -6953,8 +7165,16 @@
       <c r="AQ21" s="35"/>
       <c r="AR21" s="35"/>
       <c r="AS21" s="35"/>
-    </row>
-    <row r="22" spans="1:45" ht="15.75">
+      <c r="AT21" s="20"/>
+      <c r="AU21" s="20"/>
+      <c r="AV21" s="20"/>
+      <c r="AW21" s="20"/>
+      <c r="AX21" s="20"/>
+      <c r="AY21" s="20"/>
+      <c r="AZ21" s="20"/>
+      <c r="BA21" s="20"/>
+    </row>
+    <row r="22" spans="1:53" ht="15.75">
       <c r="A22" s="20" t="s">
         <v>302</v>
       </c>
@@ -6990,7 +7210,7 @@
       <c r="Y22" s="9"/>
       <c r="Z22" s="9"/>
       <c r="AA22" s="38" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="AB22" s="38"/>
       <c r="AC22" s="20"/>
@@ -7010,8 +7230,16 @@
       <c r="AQ22" s="35"/>
       <c r="AR22" s="35"/>
       <c r="AS22" s="35"/>
-    </row>
-    <row r="23" spans="1:45" ht="15.75">
+      <c r="AT22" s="20"/>
+      <c r="AU22" s="20"/>
+      <c r="AV22" s="20"/>
+      <c r="AW22" s="20"/>
+      <c r="AX22" s="20"/>
+      <c r="AY22" s="20"/>
+      <c r="AZ22" s="20"/>
+      <c r="BA22" s="20"/>
+    </row>
+    <row r="23" spans="1:53" ht="15.75">
       <c r="A23" s="20" t="s">
         <v>303</v>
       </c>
@@ -7047,7 +7275,7 @@
       <c r="AA23" s="38"/>
       <c r="AB23" s="38"/>
       <c r="AC23" s="20" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="AD23" s="35"/>
       <c r="AE23" s="35"/>
@@ -7065,8 +7293,16 @@
       <c r="AQ23" s="35"/>
       <c r="AR23" s="35"/>
       <c r="AS23" s="35"/>
-    </row>
-    <row r="24" spans="1:45" ht="15.75">
+      <c r="AT23" s="20"/>
+      <c r="AU23" s="20"/>
+      <c r="AV23" s="20"/>
+      <c r="AW23" s="20"/>
+      <c r="AX23" s="20"/>
+      <c r="AY23" s="20"/>
+      <c r="AZ23" s="20"/>
+      <c r="BA23" s="20"/>
+    </row>
+    <row r="24" spans="1:53" ht="15.75">
       <c r="A24" s="20" t="s">
         <v>304</v>
       </c>
@@ -7074,7 +7310,7 @@
         <v>308</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D24" s="41" t="s">
         <v>239</v>
@@ -7122,8 +7358,16 @@
       <c r="AQ24" s="35"/>
       <c r="AR24" s="35"/>
       <c r="AS24" s="35"/>
-    </row>
-    <row r="25" spans="1:45" ht="15.75">
+      <c r="AT24" s="20"/>
+      <c r="AU24" s="20"/>
+      <c r="AV24" s="20"/>
+      <c r="AW24" s="20"/>
+      <c r="AX24" s="20"/>
+      <c r="AY24" s="20"/>
+      <c r="AZ24" s="20"/>
+      <c r="BA24" s="20"/>
+    </row>
+    <row r="25" spans="1:53" ht="15.75">
       <c r="A25" s="20" t="s">
         <v>305</v>
       </c>
@@ -7175,8 +7419,16 @@
       <c r="AQ25" s="35"/>
       <c r="AR25" s="35"/>
       <c r="AS25" s="35"/>
-    </row>
-    <row r="26" spans="1:45" ht="15.75">
+      <c r="AT25" s="20"/>
+      <c r="AU25" s="20"/>
+      <c r="AV25" s="20"/>
+      <c r="AW25" s="20"/>
+      <c r="AX25" s="20"/>
+      <c r="AY25" s="20"/>
+      <c r="AZ25" s="20"/>
+      <c r="BA25" s="20"/>
+    </row>
+    <row r="26" spans="1:53" ht="15.75">
       <c r="A26" s="20" t="s">
         <v>306</v>
       </c>
@@ -7210,7 +7462,7 @@
       <c r="Y26" s="9"/>
       <c r="Z26" s="9"/>
       <c r="AA26" s="38" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="AB26" s="38"/>
       <c r="AC26" s="20"/>
@@ -7230,8 +7482,16 @@
       <c r="AQ26" s="35"/>
       <c r="AR26" s="35"/>
       <c r="AS26" s="35"/>
-    </row>
-    <row r="27" spans="1:45" ht="15.75">
+      <c r="AT26" s="20"/>
+      <c r="AU26" s="20"/>
+      <c r="AV26" s="20"/>
+      <c r="AW26" s="20"/>
+      <c r="AX26" s="20"/>
+      <c r="AY26" s="20"/>
+      <c r="AZ26" s="20"/>
+      <c r="BA26" s="20"/>
+    </row>
+    <row r="27" spans="1:53" ht="15.75">
       <c r="A27" s="20" t="s">
         <v>311</v>
       </c>
@@ -7265,7 +7525,7 @@
       <c r="Y27" s="9"/>
       <c r="Z27" s="9"/>
       <c r="AA27" s="38" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="AB27" s="38"/>
       <c r="AC27" s="20"/>
@@ -7285,8 +7545,16 @@
       <c r="AQ27" s="35"/>
       <c r="AR27" s="35"/>
       <c r="AS27" s="35"/>
-    </row>
-    <row r="28" spans="1:45" ht="15.75">
+      <c r="AT27" s="20"/>
+      <c r="AU27" s="20"/>
+      <c r="AV27" s="20"/>
+      <c r="AW27" s="20"/>
+      <c r="AX27" s="20"/>
+      <c r="AY27" s="20"/>
+      <c r="AZ27" s="20"/>
+      <c r="BA27" s="20"/>
+    </row>
+    <row r="28" spans="1:53" ht="15.75">
       <c r="A28" s="20" t="s">
         <v>314</v>
       </c>
@@ -7326,10 +7594,10 @@
         <v>360</v>
       </c>
       <c r="AE28" s="29" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="AF28" s="29" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AG28" s="35">
         <v>6</v>
@@ -7338,7 +7606,7 @@
         <v>45</v>
       </c>
       <c r="AI28" s="35" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="AJ28" s="35">
         <v>2022</v>
@@ -7354,13 +7622,21 @@
       <c r="AQ28" s="35"/>
       <c r="AR28" s="35"/>
       <c r="AS28" s="35"/>
-    </row>
-    <row r="29" spans="1:45" ht="15.75">
+      <c r="AT28" s="20"/>
+      <c r="AU28" s="20"/>
+      <c r="AV28" s="20"/>
+      <c r="AW28" s="20"/>
+      <c r="AX28" s="20"/>
+      <c r="AY28" s="20"/>
+      <c r="AZ28" s="20"/>
+      <c r="BA28" s="20"/>
+    </row>
+    <row r="29" spans="1:53" ht="15.75">
       <c r="A29" s="20" t="s">
         <v>314</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C29" s="41"/>
       <c r="D29" s="41"/>
@@ -7392,10 +7668,10 @@
       <c r="AB29" s="38"/>
       <c r="AC29" s="20"/>
       <c r="AD29" s="29" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="AE29" s="29" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="AF29" s="29" t="s">
         <v>282</v>
@@ -7407,7 +7683,7 @@
         <v>45</v>
       </c>
       <c r="AI29" s="35" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="AJ29" s="35">
         <v>2022</v>
@@ -7423,13 +7699,21 @@
       <c r="AQ29" s="35"/>
       <c r="AR29" s="35"/>
       <c r="AS29" s="35"/>
-    </row>
-    <row r="30" spans="1:45" ht="15.75">
+      <c r="AT29" s="20"/>
+      <c r="AU29" s="20"/>
+      <c r="AV29" s="20"/>
+      <c r="AW29" s="20"/>
+      <c r="AX29" s="20"/>
+      <c r="AY29" s="20"/>
+      <c r="AZ29" s="20"/>
+      <c r="BA29" s="20"/>
+    </row>
+    <row r="30" spans="1:53" ht="15.75">
       <c r="A30" s="20" t="s">
         <v>314</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C30" s="41"/>
       <c r="D30" s="41"/>
@@ -7461,13 +7745,13 @@
       <c r="AB30" s="38"/>
       <c r="AC30" s="20"/>
       <c r="AD30" s="29" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="AE30" s="29" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="AF30" s="29" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="AG30" s="35">
         <v>8</v>
@@ -7476,7 +7760,7 @@
         <v>45</v>
       </c>
       <c r="AI30" s="35" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="AJ30" s="35">
         <v>2022</v>
@@ -7492,13 +7776,21 @@
       <c r="AQ30" s="35"/>
       <c r="AR30" s="35"/>
       <c r="AS30" s="35"/>
-    </row>
-    <row r="31" spans="1:45" ht="15.75">
+      <c r="AT30" s="20"/>
+      <c r="AU30" s="20"/>
+      <c r="AV30" s="20"/>
+      <c r="AW30" s="20"/>
+      <c r="AX30" s="20"/>
+      <c r="AY30" s="20"/>
+      <c r="AZ30" s="20"/>
+      <c r="BA30" s="20"/>
+    </row>
+    <row r="31" spans="1:53" ht="15.75">
       <c r="A31" s="20" t="s">
         <v>314</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C31" s="41"/>
       <c r="D31" s="41"/>
@@ -7530,13 +7822,13 @@
       <c r="AB31" s="38"/>
       <c r="AC31" s="20"/>
       <c r="AD31" s="29" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="AE31" s="29" t="s">
+        <v>423</v>
+      </c>
+      <c r="AF31" s="29" t="s">
         <v>425</v>
-      </c>
-      <c r="AF31" s="29" t="s">
-        <v>427</v>
       </c>
       <c r="AG31" s="35">
         <v>9</v>
@@ -7545,7 +7837,7 @@
         <v>45</v>
       </c>
       <c r="AI31" s="35" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="AJ31" s="35">
         <v>2022</v>
@@ -7561,8 +7853,16 @@
       <c r="AQ31" s="35"/>
       <c r="AR31" s="35"/>
       <c r="AS31" s="35"/>
-    </row>
-    <row r="32" spans="1:45" ht="15.75">
+      <c r="AT31" s="20"/>
+      <c r="AU31" s="20"/>
+      <c r="AV31" s="20"/>
+      <c r="AW31" s="20"/>
+      <c r="AX31" s="20"/>
+      <c r="AY31" s="20"/>
+      <c r="AZ31" s="20"/>
+      <c r="BA31" s="20"/>
+    </row>
+    <row r="32" spans="1:53" ht="15.75">
       <c r="A32" s="20" t="s">
         <v>316</v>
       </c>
@@ -7610,10 +7910,10 @@
         <v>360</v>
       </c>
       <c r="AM32" s="29" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="AN32" s="29" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AO32" s="35">
         <v>6</v>
@@ -7622,7 +7922,7 @@
         <v>45</v>
       </c>
       <c r="AQ32" s="35" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="AR32" s="35">
         <v>2022</v>
@@ -7630,8 +7930,16 @@
       <c r="AS32" s="35" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="33" spans="1:45" ht="15.75">
+      <c r="AT32" s="20"/>
+      <c r="AU32" s="20"/>
+      <c r="AV32" s="20"/>
+      <c r="AW32" s="20"/>
+      <c r="AX32" s="20"/>
+      <c r="AY32" s="20"/>
+      <c r="AZ32" s="20"/>
+      <c r="BA32" s="20"/>
+    </row>
+    <row r="33" spans="1:53" ht="15.75">
       <c r="A33" s="20" t="s">
         <v>318</v>
       </c>
@@ -7665,7 +7973,7 @@
       <c r="Y33" s="9"/>
       <c r="Z33" s="9"/>
       <c r="AA33" s="38" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="AB33" s="38"/>
       <c r="AC33" s="20"/>
@@ -7687,8 +7995,16 @@
       <c r="AQ33" s="35"/>
       <c r="AR33" s="35"/>
       <c r="AS33" s="35"/>
-    </row>
-    <row r="34" spans="1:45" ht="15.75">
+      <c r="AT33" s="20"/>
+      <c r="AU33" s="20"/>
+      <c r="AV33" s="20"/>
+      <c r="AW33" s="20"/>
+      <c r="AX33" s="20"/>
+      <c r="AY33" s="20"/>
+      <c r="AZ33" s="20"/>
+      <c r="BA33" s="20"/>
+    </row>
+    <row r="34" spans="1:53" ht="15.75">
       <c r="A34" s="20" t="s">
         <v>320</v>
       </c>
@@ -7722,7 +8038,7 @@
       <c r="Y34" s="9"/>
       <c r="Z34" s="9"/>
       <c r="AA34" s="38" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="AB34" s="38"/>
       <c r="AC34" s="20"/>
@@ -7744,8 +8060,16 @@
       <c r="AQ34" s="35"/>
       <c r="AR34" s="35"/>
       <c r="AS34" s="35"/>
-    </row>
-    <row r="35" spans="1:45" ht="15.75">
+      <c r="AT34" s="20"/>
+      <c r="AU34" s="20"/>
+      <c r="AV34" s="20"/>
+      <c r="AW34" s="20"/>
+      <c r="AX34" s="20"/>
+      <c r="AY34" s="20"/>
+      <c r="AZ34" s="20"/>
+      <c r="BA34" s="20"/>
+    </row>
+    <row r="35" spans="1:53" ht="15.75">
       <c r="A35" s="20" t="s">
         <v>321</v>
       </c>
@@ -7797,8 +8121,16 @@
       <c r="AQ35" s="35"/>
       <c r="AR35" s="35"/>
       <c r="AS35" s="35"/>
-    </row>
-    <row r="36" spans="1:45" ht="15.75">
+      <c r="AT35" s="20"/>
+      <c r="AU35" s="20"/>
+      <c r="AV35" s="20"/>
+      <c r="AW35" s="20"/>
+      <c r="AX35" s="20"/>
+      <c r="AY35" s="20"/>
+      <c r="AZ35" s="20"/>
+      <c r="BA35" s="20"/>
+    </row>
+    <row r="36" spans="1:53" ht="15.75">
       <c r="A36" s="20" t="s">
         <v>324</v>
       </c>
@@ -7850,8 +8182,32 @@
       <c r="AQ36" s="35"/>
       <c r="AR36" s="35"/>
       <c r="AS36" s="35"/>
-    </row>
-    <row r="37" spans="1:45" ht="15.75">
+      <c r="AT36" s="20" t="s">
+        <v>450</v>
+      </c>
+      <c r="AU36" s="20" t="s">
+        <v>450</v>
+      </c>
+      <c r="AV36" s="20" t="s">
+        <v>450</v>
+      </c>
+      <c r="AW36" s="20" t="s">
+        <v>451</v>
+      </c>
+      <c r="AX36" s="20" t="s">
+        <v>449</v>
+      </c>
+      <c r="AY36" s="20" t="s">
+        <v>448</v>
+      </c>
+      <c r="AZ36" s="20">
+        <v>10</v>
+      </c>
+      <c r="BA36" s="20">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:53" ht="15.75">
       <c r="A37" s="20" t="s">
         <v>326</v>
       </c>
@@ -7903,8 +8259,16 @@
       <c r="AQ37" s="35"/>
       <c r="AR37" s="35"/>
       <c r="AS37" s="35"/>
-    </row>
-    <row r="38" spans="1:45" ht="15.75">
+      <c r="AT37" s="20"/>
+      <c r="AU37" s="20"/>
+      <c r="AV37" s="20"/>
+      <c r="AW37" s="20"/>
+      <c r="AX37" s="20"/>
+      <c r="AY37" s="20"/>
+      <c r="AZ37" s="20"/>
+      <c r="BA37" s="20"/>
+    </row>
+    <row r="38" spans="1:53" ht="15.75">
       <c r="A38" s="20" t="s">
         <v>328</v>
       </c>
@@ -7956,8 +8320,16 @@
       <c r="AQ38" s="35"/>
       <c r="AR38" s="35"/>
       <c r="AS38" s="35"/>
-    </row>
-    <row r="39" spans="1:45" ht="15.75">
+      <c r="AT38" s="20"/>
+      <c r="AU38" s="20"/>
+      <c r="AV38" s="20"/>
+      <c r="AW38" s="20"/>
+      <c r="AX38" s="20"/>
+      <c r="AY38" s="20"/>
+      <c r="AZ38" s="20"/>
+      <c r="BA38" s="20"/>
+    </row>
+    <row r="39" spans="1:53" ht="15.75">
       <c r="A39" s="20" t="s">
         <v>329</v>
       </c>
@@ -8009,8 +8381,16 @@
       <c r="AQ39" s="35"/>
       <c r="AR39" s="35"/>
       <c r="AS39" s="35"/>
-    </row>
-    <row r="40" spans="1:45" ht="15.75">
+      <c r="AT39" s="20"/>
+      <c r="AU39" s="20"/>
+      <c r="AV39" s="20"/>
+      <c r="AW39" s="20"/>
+      <c r="AX39" s="20"/>
+      <c r="AY39" s="20"/>
+      <c r="AZ39" s="20"/>
+      <c r="BA39" s="20"/>
+    </row>
+    <row r="40" spans="1:53" ht="15.75">
       <c r="A40" s="20" t="s">
         <v>332</v>
       </c>
@@ -8062,8 +8442,16 @@
       <c r="AQ40" s="35"/>
       <c r="AR40" s="35"/>
       <c r="AS40" s="35"/>
-    </row>
-    <row r="41" spans="1:45" ht="15.75">
+      <c r="AT40" s="20"/>
+      <c r="AU40" s="20"/>
+      <c r="AV40" s="20"/>
+      <c r="AW40" s="20"/>
+      <c r="AX40" s="20"/>
+      <c r="AY40" s="20"/>
+      <c r="AZ40" s="20"/>
+      <c r="BA40" s="20"/>
+    </row>
+    <row r="41" spans="1:53" ht="15.75">
       <c r="A41" s="20" t="s">
         <v>333</v>
       </c>
@@ -8115,8 +8503,16 @@
       <c r="AQ41" s="35"/>
       <c r="AR41" s="35"/>
       <c r="AS41" s="35"/>
-    </row>
-    <row r="42" spans="1:45" ht="15.75">
+      <c r="AT41" s="20"/>
+      <c r="AU41" s="20"/>
+      <c r="AV41" s="20"/>
+      <c r="AW41" s="20"/>
+      <c r="AX41" s="20"/>
+      <c r="AY41" s="20"/>
+      <c r="AZ41" s="20"/>
+      <c r="BA41" s="20"/>
+    </row>
+    <row r="42" spans="1:53" ht="15.75">
       <c r="A42" s="20" t="s">
         <v>336</v>
       </c>
@@ -8168,8 +8564,16 @@
       <c r="AQ42" s="35"/>
       <c r="AR42" s="35"/>
       <c r="AS42" s="35"/>
-    </row>
-    <row r="43" spans="1:45" ht="15.75">
+      <c r="AT42" s="20"/>
+      <c r="AU42" s="20"/>
+      <c r="AV42" s="20"/>
+      <c r="AW42" s="20"/>
+      <c r="AX42" s="20"/>
+      <c r="AY42" s="20"/>
+      <c r="AZ42" s="20"/>
+      <c r="BA42" s="20"/>
+    </row>
+    <row r="43" spans="1:53" ht="15.75">
       <c r="A43" s="20" t="s">
         <v>337</v>
       </c>
@@ -8221,8 +8625,16 @@
       <c r="AQ43" s="35"/>
       <c r="AR43" s="35"/>
       <c r="AS43" s="35"/>
-    </row>
-    <row r="44" spans="1:45" ht="15.75">
+      <c r="AT43" s="20"/>
+      <c r="AU43" s="20"/>
+      <c r="AV43" s="20"/>
+      <c r="AW43" s="20"/>
+      <c r="AX43" s="20"/>
+      <c r="AY43" s="20"/>
+      <c r="AZ43" s="20"/>
+      <c r="BA43" s="20"/>
+    </row>
+    <row r="44" spans="1:53" ht="15.75">
       <c r="A44" s="20" t="s">
         <v>340</v>
       </c>
@@ -8274,8 +8686,16 @@
       <c r="AQ44" s="35"/>
       <c r="AR44" s="35"/>
       <c r="AS44" s="35"/>
-    </row>
-    <row r="45" spans="1:45" ht="15.75">
+      <c r="AT44" s="20"/>
+      <c r="AU44" s="20"/>
+      <c r="AV44" s="20"/>
+      <c r="AW44" s="20"/>
+      <c r="AX44" s="20"/>
+      <c r="AY44" s="20"/>
+      <c r="AZ44" s="20"/>
+      <c r="BA44" s="20"/>
+    </row>
+    <row r="45" spans="1:53" ht="15.75">
       <c r="A45" s="20" t="s">
         <v>341</v>
       </c>
@@ -8327,8 +8747,16 @@
       <c r="AQ45" s="35"/>
       <c r="AR45" s="35"/>
       <c r="AS45" s="35"/>
-    </row>
-    <row r="46" spans="1:45" ht="15.75">
+      <c r="AT45" s="20"/>
+      <c r="AU45" s="20"/>
+      <c r="AV45" s="20"/>
+      <c r="AW45" s="20"/>
+      <c r="AX45" s="20"/>
+      <c r="AY45" s="20"/>
+      <c r="AZ45" s="20"/>
+      <c r="BA45" s="20"/>
+    </row>
+    <row r="46" spans="1:53" ht="15.75">
       <c r="A46" s="20" t="s">
         <v>344</v>
       </c>
@@ -8380,8 +8808,16 @@
       <c r="AQ46" s="35"/>
       <c r="AR46" s="35"/>
       <c r="AS46" s="35"/>
-    </row>
-    <row r="47" spans="1:45" ht="15.75">
+      <c r="AT46" s="20"/>
+      <c r="AU46" s="20"/>
+      <c r="AV46" s="20"/>
+      <c r="AW46" s="20"/>
+      <c r="AX46" s="20"/>
+      <c r="AY46" s="20"/>
+      <c r="AZ46" s="20"/>
+      <c r="BA46" s="20"/>
+    </row>
+    <row r="47" spans="1:53" ht="15.75">
       <c r="A47" s="20" t="s">
         <v>345</v>
       </c>
@@ -8433,8 +8869,16 @@
       <c r="AQ47" s="35"/>
       <c r="AR47" s="35"/>
       <c r="AS47" s="35"/>
-    </row>
-    <row r="48" spans="1:45" ht="15.75">
+      <c r="AT47" s="20"/>
+      <c r="AU47" s="20"/>
+      <c r="AV47" s="20"/>
+      <c r="AW47" s="20"/>
+      <c r="AX47" s="20"/>
+      <c r="AY47" s="20"/>
+      <c r="AZ47" s="20"/>
+      <c r="BA47" s="20"/>
+    </row>
+    <row r="48" spans="1:53" ht="15.75">
       <c r="A48" s="20" t="s">
         <v>346</v>
       </c>
@@ -8486,6 +8930,14 @@
       <c r="AQ48" s="35"/>
       <c r="AR48" s="35"/>
       <c r="AS48" s="35"/>
+      <c r="AT48" s="20"/>
+      <c r="AU48" s="20"/>
+      <c r="AV48" s="20"/>
+      <c r="AW48" s="20"/>
+      <c r="AX48" s="20"/>
+      <c r="AY48" s="20"/>
+      <c r="AZ48" s="20"/>
+      <c r="BA48" s="20"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
commit gl2 report test cases
</commit_message>
<xml_diff>
--- a/Ajith_KUBS_CEN_GeneralLedger12/Test-data/GLTestData.xlsx
+++ b/Ajith_KUBS_CEN_GeneralLedger12/Test-data/GLTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AllMastersTestDataInfo" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="453">
   <si>
     <t>Creation of Asset AutoMaster</t>
   </si>
@@ -1378,6 +1378,9 @@
   </si>
   <si>
     <t>TestModule</t>
+  </si>
+  <si>
+    <t>ReportType</t>
   </si>
 </sst>
 </file>
@@ -1528,7 +1531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1624,6 +1627,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5632,10 +5638,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BM48"/>
+  <dimension ref="A1:BN48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="AW36" sqref="AW36"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="V1" sqref="V1"/>
+      <selection pane="bottomLeft" activeCell="P42" sqref="P42:R42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.28515625" defaultRowHeight="15"/>
@@ -5651,13 +5659,13 @@
     <col min="13" max="13" width="38.85546875" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="49.5703125" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="44.42578125" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="36.42578125" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="53.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="36.42578125" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="37.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65">
+    <row r="1" spans="1:66">
       <c r="A1" s="19" t="s">
         <v>23</v>
       </c>
@@ -5706,118 +5714,120 @@
       <c r="P1" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="18" t="s">
+        <v>452</v>
+      </c>
+      <c r="R1" s="19" t="s">
         <v>362</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>363</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="T1" s="19" t="s">
         <v>364</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="U1" s="19" t="s">
         <v>365</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="V1" s="19" t="s">
         <v>366</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="W1" s="19" t="s">
         <v>367</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="X1" s="18" t="s">
         <v>368</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>369</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Z1" s="19" t="s">
         <v>370</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AB1" s="19" t="s">
         <v>377</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AC1" s="19" t="s">
         <v>434</v>
       </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AD1" s="19" t="s">
         <v>407</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AE1" s="19" t="s">
         <v>409</v>
       </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AF1" s="19" t="s">
         <v>410</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AG1" s="19" t="s">
         <v>411</v>
       </c>
-      <c r="AG1" s="19" t="s">
+      <c r="AH1" s="19" t="s">
         <v>412</v>
       </c>
-      <c r="AH1" s="19" t="s">
+      <c r="AI1" s="19" t="s">
         <v>413</v>
       </c>
-      <c r="AI1" s="19" t="s">
+      <c r="AJ1" s="19" t="s">
         <v>414</v>
       </c>
-      <c r="AJ1" s="19" t="s">
+      <c r="AK1" s="19" t="s">
         <v>415</v>
       </c>
-      <c r="AK1" s="19" t="s">
+      <c r="AL1" s="19" t="s">
         <v>435</v>
       </c>
-      <c r="AL1" s="19" t="s">
+      <c r="AM1" s="19" t="s">
         <v>427</v>
       </c>
-      <c r="AM1" s="19" t="s">
+      <c r="AN1" s="19" t="s">
         <v>428</v>
       </c>
-      <c r="AN1" s="19" t="s">
+      <c r="AO1" s="19" t="s">
         <v>429</v>
       </c>
-      <c r="AO1" s="19" t="s">
+      <c r="AP1" s="19" t="s">
         <v>430</v>
       </c>
-      <c r="AP1" s="19" t="s">
+      <c r="AQ1" s="19" t="s">
         <v>431</v>
       </c>
-      <c r="AQ1" s="19" t="s">
+      <c r="AR1" s="19" t="s">
         <v>432</v>
       </c>
-      <c r="AR1" s="19" t="s">
+      <c r="AS1" s="19" t="s">
         <v>433</v>
       </c>
-      <c r="AS1" s="19" t="s">
+      <c r="AT1" s="19" t="s">
         <v>436</v>
       </c>
-      <c r="AT1" s="19" t="s">
+      <c r="AU1" s="19" t="s">
         <v>440</v>
       </c>
-      <c r="AU1" s="19" t="s">
+      <c r="AV1" s="19" t="s">
         <v>441</v>
       </c>
-      <c r="AV1" s="19" t="s">
+      <c r="AW1" s="19" t="s">
         <v>442</v>
       </c>
-      <c r="AW1" s="19" t="s">
+      <c r="AX1" s="19" t="s">
         <v>443</v>
       </c>
-      <c r="AX1" s="19" t="s">
+      <c r="AY1" s="19" t="s">
         <v>444</v>
       </c>
-      <c r="AY1" s="19" t="s">
+      <c r="AZ1" s="19" t="s">
         <v>445</v>
       </c>
-      <c r="AZ1" s="19" t="s">
+      <c r="BA1" s="19" t="s">
         <v>446</v>
       </c>
-      <c r="BA1" s="19" t="s">
+      <c r="BB1" s="19" t="s">
         <v>447</v>
       </c>
-      <c r="BB1" s="19"/>
       <c r="BC1" s="19"/>
       <c r="BD1" s="19"/>
       <c r="BE1" s="19"/>
@@ -5829,8 +5839,9 @@
       <c r="BK1" s="19"/>
       <c r="BL1" s="19"/>
       <c r="BM1" s="19"/>
-    </row>
-    <row r="2" spans="1:65" ht="15.75">
+      <c r="BN1" s="19"/>
+    </row>
+    <row r="2" spans="1:66" ht="15.75">
       <c r="A2" s="20" t="s">
         <v>248</v>
       </c>
@@ -5875,22 +5886,22 @@
         <v>284</v>
       </c>
       <c r="P2" s="34"/>
-      <c r="Q2" s="9"/>
+      <c r="Q2" s="34"/>
       <c r="R2" s="9"/>
-      <c r="S2" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U2" s="9"/>
       <c r="V2" s="9"/>
       <c r="W2" s="9"/>
       <c r="X2" s="9"/>
       <c r="Y2" s="9"/>
       <c r="Z2" s="9"/>
-      <c r="AA2" s="38"/>
+      <c r="AA2" s="9"/>
       <c r="AB2" s="38"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="35"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="20"/>
       <c r="AE2" s="35"/>
       <c r="AF2" s="35"/>
       <c r="AG2" s="35"/>
@@ -5899,23 +5910,24 @@
       <c r="AJ2" s="35"/>
       <c r="AK2" s="35"/>
       <c r="AL2" s="35"/>
-      <c r="AM2" s="35"/>
-      <c r="AN2" s="35"/>
+      <c r="AM2" s="49"/>
+      <c r="AN2" s="49"/>
       <c r="AO2" s="35"/>
       <c r="AP2" s="35"/>
       <c r="AQ2" s="35"/>
       <c r="AR2" s="35"/>
       <c r="AS2" s="35"/>
-      <c r="AT2" s="20"/>
+      <c r="AT2" s="35"/>
       <c r="AU2" s="20"/>
       <c r="AV2" s="20"/>
       <c r="AW2" s="20"/>
       <c r="AX2" s="20"/>
-      <c r="AY2" s="20"/>
-      <c r="AZ2" s="20"/>
+      <c r="AY2" s="27"/>
+      <c r="AZ2" s="27"/>
       <c r="BA2" s="20"/>
-    </row>
-    <row r="3" spans="1:65" ht="15.75">
+      <c r="BB2" s="20"/>
+    </row>
+    <row r="3" spans="1:66" ht="15.75">
       <c r="A3" s="20" t="s">
         <v>260</v>
       </c>
@@ -5940,22 +5952,22 @@
       <c r="N3" s="34"/>
       <c r="O3" s="34"/>
       <c r="P3" s="34"/>
-      <c r="Q3" s="9"/>
+      <c r="Q3" s="34"/>
       <c r="R3" s="9"/>
-      <c r="S3" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U3" s="9"/>
       <c r="V3" s="9"/>
       <c r="W3" s="9"/>
       <c r="X3" s="9"/>
       <c r="Y3" s="9"/>
       <c r="Z3" s="9"/>
-      <c r="AA3" s="38"/>
+      <c r="AA3" s="9"/>
       <c r="AB3" s="38"/>
-      <c r="AC3" s="20"/>
-      <c r="AD3" s="35"/>
+      <c r="AC3" s="38"/>
+      <c r="AD3" s="20"/>
       <c r="AE3" s="35"/>
       <c r="AF3" s="35"/>
       <c r="AG3" s="35"/>
@@ -5964,23 +5976,24 @@
       <c r="AJ3" s="35"/>
       <c r="AK3" s="35"/>
       <c r="AL3" s="35"/>
-      <c r="AM3" s="35"/>
-      <c r="AN3" s="35"/>
+      <c r="AM3" s="49"/>
+      <c r="AN3" s="49"/>
       <c r="AO3" s="35"/>
       <c r="AP3" s="35"/>
       <c r="AQ3" s="35"/>
       <c r="AR3" s="35"/>
       <c r="AS3" s="35"/>
-      <c r="AT3" s="20"/>
+      <c r="AT3" s="35"/>
       <c r="AU3" s="20"/>
       <c r="AV3" s="20"/>
       <c r="AW3" s="20"/>
       <c r="AX3" s="20"/>
-      <c r="AY3" s="20"/>
-      <c r="AZ3" s="20"/>
+      <c r="AY3" s="27"/>
+      <c r="AZ3" s="27"/>
       <c r="BA3" s="20"/>
-    </row>
-    <row r="4" spans="1:65" ht="15.75">
+      <c r="BB3" s="20"/>
+    </row>
+    <row r="4" spans="1:66" ht="15.75">
       <c r="A4" s="20" t="s">
         <v>261</v>
       </c>
@@ -6001,22 +6014,22 @@
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
       <c r="P4" s="34"/>
-      <c r="Q4" s="9"/>
+      <c r="Q4" s="34"/>
       <c r="R4" s="9"/>
-      <c r="S4" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U4" s="9"/>
       <c r="V4" s="9"/>
       <c r="W4" s="9"/>
       <c r="X4" s="9"/>
       <c r="Y4" s="9"/>
       <c r="Z4" s="9"/>
-      <c r="AA4" s="38"/>
+      <c r="AA4" s="9"/>
       <c r="AB4" s="38"/>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="35"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="20"/>
       <c r="AE4" s="35"/>
       <c r="AF4" s="35"/>
       <c r="AG4" s="35"/>
@@ -6025,23 +6038,24 @@
       <c r="AJ4" s="35"/>
       <c r="AK4" s="35"/>
       <c r="AL4" s="35"/>
-      <c r="AM4" s="35"/>
-      <c r="AN4" s="35"/>
+      <c r="AM4" s="49"/>
+      <c r="AN4" s="49"/>
       <c r="AO4" s="35"/>
       <c r="AP4" s="35"/>
       <c r="AQ4" s="35"/>
       <c r="AR4" s="35"/>
       <c r="AS4" s="35"/>
-      <c r="AT4" s="20"/>
+      <c r="AT4" s="35"/>
       <c r="AU4" s="20"/>
       <c r="AV4" s="20"/>
       <c r="AW4" s="20"/>
       <c r="AX4" s="20"/>
-      <c r="AY4" s="20"/>
-      <c r="AZ4" s="20"/>
+      <c r="AY4" s="27"/>
+      <c r="AZ4" s="27"/>
       <c r="BA4" s="20"/>
-    </row>
-    <row r="5" spans="1:65" ht="15.75">
+      <c r="BB4" s="20"/>
+    </row>
+    <row r="5" spans="1:66" ht="15.75">
       <c r="A5" s="20" t="s">
         <v>262</v>
       </c>
@@ -6062,22 +6076,22 @@
       <c r="N5" s="34"/>
       <c r="O5" s="34"/>
       <c r="P5" s="34"/>
-      <c r="Q5" s="9"/>
+      <c r="Q5" s="34"/>
       <c r="R5" s="9"/>
-      <c r="S5" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U5" s="9"/>
       <c r="V5" s="9"/>
       <c r="W5" s="9"/>
       <c r="X5" s="9"/>
       <c r="Y5" s="9"/>
       <c r="Z5" s="9"/>
-      <c r="AA5" s="38"/>
+      <c r="AA5" s="9"/>
       <c r="AB5" s="38"/>
-      <c r="AC5" s="20"/>
-      <c r="AD5" s="35"/>
+      <c r="AC5" s="38"/>
+      <c r="AD5" s="20"/>
       <c r="AE5" s="35"/>
       <c r="AF5" s="35"/>
       <c r="AG5" s="35"/>
@@ -6086,23 +6100,24 @@
       <c r="AJ5" s="35"/>
       <c r="AK5" s="35"/>
       <c r="AL5" s="35"/>
-      <c r="AM5" s="35"/>
-      <c r="AN5" s="35"/>
+      <c r="AM5" s="49"/>
+      <c r="AN5" s="49"/>
       <c r="AO5" s="35"/>
       <c r="AP5" s="35"/>
       <c r="AQ5" s="35"/>
       <c r="AR5" s="35"/>
       <c r="AS5" s="35"/>
-      <c r="AT5" s="20"/>
+      <c r="AT5" s="35"/>
       <c r="AU5" s="20"/>
       <c r="AV5" s="20"/>
       <c r="AW5" s="20"/>
       <c r="AX5" s="20"/>
-      <c r="AY5" s="20"/>
-      <c r="AZ5" s="20"/>
+      <c r="AY5" s="27"/>
+      <c r="AZ5" s="27"/>
       <c r="BA5" s="20"/>
-    </row>
-    <row r="6" spans="1:65" ht="15.75">
+      <c r="BB5" s="20"/>
+    </row>
+    <row r="6" spans="1:66" ht="15.75">
       <c r="A6" s="20" t="s">
         <v>266</v>
       </c>
@@ -6143,22 +6158,22 @@
         <v>359</v>
       </c>
       <c r="P6" s="34"/>
-      <c r="Q6" s="9"/>
+      <c r="Q6" s="34"/>
       <c r="R6" s="9"/>
-      <c r="S6" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U6" s="9"/>
       <c r="V6" s="9"/>
       <c r="W6" s="9"/>
       <c r="X6" s="9"/>
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
-      <c r="AA6" s="38"/>
+      <c r="AA6" s="9"/>
       <c r="AB6" s="38"/>
-      <c r="AC6" s="20"/>
-      <c r="AD6" s="35"/>
+      <c r="AC6" s="38"/>
+      <c r="AD6" s="20"/>
       <c r="AE6" s="35"/>
       <c r="AF6" s="35"/>
       <c r="AG6" s="35"/>
@@ -6167,23 +6182,24 @@
       <c r="AJ6" s="35"/>
       <c r="AK6" s="35"/>
       <c r="AL6" s="35"/>
-      <c r="AM6" s="35"/>
-      <c r="AN6" s="35"/>
+      <c r="AM6" s="49"/>
+      <c r="AN6" s="49"/>
       <c r="AO6" s="35"/>
       <c r="AP6" s="35"/>
       <c r="AQ6" s="35"/>
       <c r="AR6" s="35"/>
       <c r="AS6" s="35"/>
-      <c r="AT6" s="20"/>
+      <c r="AT6" s="35"/>
       <c r="AU6" s="20"/>
       <c r="AV6" s="20"/>
       <c r="AW6" s="20"/>
       <c r="AX6" s="20"/>
-      <c r="AY6" s="20"/>
-      <c r="AZ6" s="20"/>
+      <c r="AY6" s="27"/>
+      <c r="AZ6" s="27"/>
       <c r="BA6" s="20"/>
-    </row>
-    <row r="7" spans="1:65" ht="15.75">
+      <c r="BB6" s="20"/>
+    </row>
+    <row r="7" spans="1:66" ht="15.75">
       <c r="A7" s="20" t="s">
         <v>271</v>
       </c>
@@ -6208,22 +6224,22 @@
       <c r="N7" s="34"/>
       <c r="O7" s="34"/>
       <c r="P7" s="34"/>
-      <c r="Q7" s="9"/>
+      <c r="Q7" s="34"/>
       <c r="R7" s="9"/>
-      <c r="S7" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U7" s="9"/>
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
       <c r="X7" s="9"/>
       <c r="Y7" s="9"/>
       <c r="Z7" s="9"/>
-      <c r="AA7" s="38"/>
+      <c r="AA7" s="9"/>
       <c r="AB7" s="38"/>
-      <c r="AC7" s="20"/>
-      <c r="AD7" s="35"/>
+      <c r="AC7" s="38"/>
+      <c r="AD7" s="20"/>
       <c r="AE7" s="35"/>
       <c r="AF7" s="35"/>
       <c r="AG7" s="35"/>
@@ -6232,23 +6248,24 @@
       <c r="AJ7" s="35"/>
       <c r="AK7" s="35"/>
       <c r="AL7" s="35"/>
-      <c r="AM7" s="35"/>
-      <c r="AN7" s="35"/>
+      <c r="AM7" s="49"/>
+      <c r="AN7" s="49"/>
       <c r="AO7" s="35"/>
       <c r="AP7" s="35"/>
       <c r="AQ7" s="35"/>
       <c r="AR7" s="35"/>
       <c r="AS7" s="35"/>
-      <c r="AT7" s="20"/>
+      <c r="AT7" s="35"/>
       <c r="AU7" s="20"/>
       <c r="AV7" s="20"/>
       <c r="AW7" s="20"/>
       <c r="AX7" s="20"/>
-      <c r="AY7" s="20"/>
-      <c r="AZ7" s="20"/>
+      <c r="AY7" s="27"/>
+      <c r="AZ7" s="27"/>
       <c r="BA7" s="20"/>
-    </row>
-    <row r="8" spans="1:65" ht="15.75">
+      <c r="BB7" s="20"/>
+    </row>
+    <row r="8" spans="1:66" ht="15.75">
       <c r="A8" s="20" t="s">
         <v>272</v>
       </c>
@@ -6269,22 +6286,22 @@
       <c r="N8" s="34"/>
       <c r="O8" s="34"/>
       <c r="P8" s="34"/>
-      <c r="Q8" s="9"/>
+      <c r="Q8" s="34"/>
       <c r="R8" s="9"/>
-      <c r="S8" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U8" s="9"/>
       <c r="V8" s="9"/>
       <c r="W8" s="9"/>
       <c r="X8" s="9"/>
       <c r="Y8" s="9"/>
       <c r="Z8" s="9"/>
-      <c r="AA8" s="38"/>
+      <c r="AA8" s="9"/>
       <c r="AB8" s="38"/>
-      <c r="AC8" s="20"/>
-      <c r="AD8" s="35"/>
+      <c r="AC8" s="38"/>
+      <c r="AD8" s="20"/>
       <c r="AE8" s="35"/>
       <c r="AF8" s="35"/>
       <c r="AG8" s="35"/>
@@ -6293,23 +6310,24 @@
       <c r="AJ8" s="35"/>
       <c r="AK8" s="35"/>
       <c r="AL8" s="35"/>
-      <c r="AM8" s="35"/>
-      <c r="AN8" s="35"/>
+      <c r="AM8" s="49"/>
+      <c r="AN8" s="49"/>
       <c r="AO8" s="35"/>
       <c r="AP8" s="35"/>
       <c r="AQ8" s="35"/>
       <c r="AR8" s="35"/>
       <c r="AS8" s="35"/>
-      <c r="AT8" s="20"/>
+      <c r="AT8" s="35"/>
       <c r="AU8" s="20"/>
       <c r="AV8" s="20"/>
       <c r="AW8" s="20"/>
       <c r="AX8" s="20"/>
-      <c r="AY8" s="20"/>
-      <c r="AZ8" s="20"/>
+      <c r="AY8" s="27"/>
+      <c r="AZ8" s="27"/>
       <c r="BA8" s="20"/>
-    </row>
-    <row r="9" spans="1:65" ht="15.75">
+      <c r="BB8" s="20"/>
+    </row>
+    <row r="9" spans="1:66" ht="15.75">
       <c r="A9" s="20" t="s">
         <v>273</v>
       </c>
@@ -6330,22 +6348,22 @@
       <c r="N9" s="34"/>
       <c r="O9" s="34"/>
       <c r="P9" s="34"/>
-      <c r="Q9" s="9"/>
+      <c r="Q9" s="34"/>
       <c r="R9" s="9"/>
-      <c r="S9" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U9" s="9"/>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
       <c r="X9" s="9"/>
       <c r="Y9" s="9"/>
       <c r="Z9" s="9"/>
-      <c r="AA9" s="38"/>
+      <c r="AA9" s="9"/>
       <c r="AB9" s="38"/>
-      <c r="AC9" s="20"/>
-      <c r="AD9" s="35"/>
+      <c r="AC9" s="38"/>
+      <c r="AD9" s="20"/>
       <c r="AE9" s="35"/>
       <c r="AF9" s="35"/>
       <c r="AG9" s="35"/>
@@ -6354,23 +6372,24 @@
       <c r="AJ9" s="35"/>
       <c r="AK9" s="35"/>
       <c r="AL9" s="35"/>
-      <c r="AM9" s="35"/>
-      <c r="AN9" s="35"/>
+      <c r="AM9" s="49"/>
+      <c r="AN9" s="49"/>
       <c r="AO9" s="35"/>
       <c r="AP9" s="35"/>
       <c r="AQ9" s="35"/>
       <c r="AR9" s="35"/>
       <c r="AS9" s="35"/>
-      <c r="AT9" s="20"/>
+      <c r="AT9" s="35"/>
       <c r="AU9" s="20"/>
       <c r="AV9" s="20"/>
       <c r="AW9" s="20"/>
       <c r="AX9" s="20"/>
-      <c r="AY9" s="20"/>
-      <c r="AZ9" s="20"/>
+      <c r="AY9" s="27"/>
+      <c r="AZ9" s="27"/>
       <c r="BA9" s="20"/>
-    </row>
-    <row r="10" spans="1:65" ht="15.75">
+      <c r="BB9" s="20"/>
+    </row>
+    <row r="10" spans="1:66" ht="15.75">
       <c r="A10" s="20" t="s">
         <v>274</v>
       </c>
@@ -6411,22 +6430,22 @@
         <v>350</v>
       </c>
       <c r="P10" s="34"/>
-      <c r="Q10" s="9"/>
+      <c r="Q10" s="34"/>
       <c r="R10" s="9"/>
-      <c r="S10" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U10" s="9"/>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
       <c r="X10" s="9"/>
       <c r="Y10" s="9"/>
       <c r="Z10" s="9"/>
-      <c r="AA10" s="38"/>
+      <c r="AA10" s="9"/>
       <c r="AB10" s="38"/>
-      <c r="AC10" s="20"/>
-      <c r="AD10" s="35"/>
+      <c r="AC10" s="38"/>
+      <c r="AD10" s="20"/>
       <c r="AE10" s="35"/>
       <c r="AF10" s="35"/>
       <c r="AG10" s="35"/>
@@ -6435,23 +6454,24 @@
       <c r="AJ10" s="35"/>
       <c r="AK10" s="35"/>
       <c r="AL10" s="35"/>
-      <c r="AM10" s="35"/>
-      <c r="AN10" s="35"/>
+      <c r="AM10" s="49"/>
+      <c r="AN10" s="49"/>
       <c r="AO10" s="35"/>
       <c r="AP10" s="35"/>
       <c r="AQ10" s="35"/>
       <c r="AR10" s="35"/>
       <c r="AS10" s="35"/>
-      <c r="AT10" s="20"/>
+      <c r="AT10" s="35"/>
       <c r="AU10" s="20"/>
       <c r="AV10" s="20"/>
       <c r="AW10" s="20"/>
       <c r="AX10" s="20"/>
-      <c r="AY10" s="20"/>
-      <c r="AZ10" s="20"/>
+      <c r="AY10" s="27"/>
+      <c r="AZ10" s="27"/>
       <c r="BA10" s="20"/>
-    </row>
-    <row r="11" spans="1:65" ht="15.75">
+      <c r="BB10" s="20"/>
+    </row>
+    <row r="11" spans="1:66" ht="15.75">
       <c r="A11" s="20" t="s">
         <v>275</v>
       </c>
@@ -6476,22 +6496,22 @@
       <c r="N11" s="34"/>
       <c r="O11" s="34"/>
       <c r="P11" s="34"/>
-      <c r="Q11" s="9"/>
+      <c r="Q11" s="34"/>
       <c r="R11" s="9"/>
-      <c r="S11" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U11" s="9"/>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
       <c r="Z11" s="9"/>
-      <c r="AA11" s="38"/>
+      <c r="AA11" s="9"/>
       <c r="AB11" s="38"/>
-      <c r="AC11" s="20"/>
-      <c r="AD11" s="35"/>
+      <c r="AC11" s="38"/>
+      <c r="AD11" s="20"/>
       <c r="AE11" s="35"/>
       <c r="AF11" s="35"/>
       <c r="AG11" s="35"/>
@@ -6500,23 +6520,24 @@
       <c r="AJ11" s="35"/>
       <c r="AK11" s="35"/>
       <c r="AL11" s="35"/>
-      <c r="AM11" s="35"/>
-      <c r="AN11" s="35"/>
+      <c r="AM11" s="49"/>
+      <c r="AN11" s="49"/>
       <c r="AO11" s="35"/>
       <c r="AP11" s="35"/>
       <c r="AQ11" s="35"/>
       <c r="AR11" s="35"/>
       <c r="AS11" s="35"/>
-      <c r="AT11" s="20"/>
+      <c r="AT11" s="35"/>
       <c r="AU11" s="20"/>
       <c r="AV11" s="20"/>
       <c r="AW11" s="20"/>
       <c r="AX11" s="20"/>
-      <c r="AY11" s="20"/>
-      <c r="AZ11" s="20"/>
+      <c r="AY11" s="27"/>
+      <c r="AZ11" s="27"/>
       <c r="BA11" s="20"/>
-    </row>
-    <row r="12" spans="1:65" ht="15.75">
+      <c r="BB11" s="20"/>
+    </row>
+    <row r="12" spans="1:66" ht="15.75">
       <c r="A12" s="20" t="s">
         <v>276</v>
       </c>
@@ -6537,22 +6558,22 @@
       <c r="N12" s="34"/>
       <c r="O12" s="34"/>
       <c r="P12" s="34"/>
-      <c r="Q12" s="9"/>
+      <c r="Q12" s="34"/>
       <c r="R12" s="9"/>
-      <c r="S12" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U12" s="9"/>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
       <c r="X12" s="9"/>
       <c r="Y12" s="9"/>
       <c r="Z12" s="9"/>
-      <c r="AA12" s="38"/>
+      <c r="AA12" s="9"/>
       <c r="AB12" s="38"/>
-      <c r="AC12" s="20"/>
-      <c r="AD12" s="35"/>
+      <c r="AC12" s="38"/>
+      <c r="AD12" s="20"/>
       <c r="AE12" s="35"/>
       <c r="AF12" s="35"/>
       <c r="AG12" s="35"/>
@@ -6561,23 +6582,24 @@
       <c r="AJ12" s="35"/>
       <c r="AK12" s="35"/>
       <c r="AL12" s="35"/>
-      <c r="AM12" s="35"/>
-      <c r="AN12" s="35"/>
+      <c r="AM12" s="49"/>
+      <c r="AN12" s="49"/>
       <c r="AO12" s="35"/>
       <c r="AP12" s="35"/>
       <c r="AQ12" s="35"/>
       <c r="AR12" s="35"/>
       <c r="AS12" s="35"/>
-      <c r="AT12" s="20"/>
+      <c r="AT12" s="35"/>
       <c r="AU12" s="20"/>
       <c r="AV12" s="20"/>
       <c r="AW12" s="20"/>
       <c r="AX12" s="20"/>
-      <c r="AY12" s="20"/>
-      <c r="AZ12" s="20"/>
+      <c r="AY12" s="27"/>
+      <c r="AZ12" s="27"/>
       <c r="BA12" s="20"/>
-    </row>
-    <row r="13" spans="1:65" ht="15.75">
+      <c r="BB12" s="20"/>
+    </row>
+    <row r="13" spans="1:66" ht="15.75">
       <c r="A13" s="20" t="s">
         <v>277</v>
       </c>
@@ -6598,22 +6620,22 @@
       <c r="N13" s="34"/>
       <c r="O13" s="34"/>
       <c r="P13" s="34"/>
-      <c r="Q13" s="9"/>
+      <c r="Q13" s="34"/>
       <c r="R13" s="9"/>
-      <c r="S13" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U13" s="9"/>
       <c r="V13" s="9"/>
       <c r="W13" s="9"/>
       <c r="X13" s="9"/>
       <c r="Y13" s="9"/>
       <c r="Z13" s="9"/>
-      <c r="AA13" s="38"/>
+      <c r="AA13" s="9"/>
       <c r="AB13" s="38"/>
-      <c r="AC13" s="20"/>
-      <c r="AD13" s="35"/>
+      <c r="AC13" s="38"/>
+      <c r="AD13" s="20"/>
       <c r="AE13" s="35"/>
       <c r="AF13" s="35"/>
       <c r="AG13" s="35"/>
@@ -6622,23 +6644,24 @@
       <c r="AJ13" s="35"/>
       <c r="AK13" s="35"/>
       <c r="AL13" s="35"/>
-      <c r="AM13" s="35"/>
-      <c r="AN13" s="35"/>
+      <c r="AM13" s="49"/>
+      <c r="AN13" s="49"/>
       <c r="AO13" s="35"/>
       <c r="AP13" s="35"/>
       <c r="AQ13" s="35"/>
       <c r="AR13" s="35"/>
       <c r="AS13" s="35"/>
-      <c r="AT13" s="20"/>
+      <c r="AT13" s="35"/>
       <c r="AU13" s="20"/>
       <c r="AV13" s="20"/>
       <c r="AW13" s="20"/>
       <c r="AX13" s="20"/>
-      <c r="AY13" s="20"/>
-      <c r="AZ13" s="20"/>
+      <c r="AY13" s="27"/>
+      <c r="AZ13" s="27"/>
       <c r="BA13" s="20"/>
-    </row>
-    <row r="14" spans="1:65" ht="15.75">
+      <c r="BB13" s="20"/>
+    </row>
+    <row r="14" spans="1:66" ht="15.75">
       <c r="A14" s="20" t="s">
         <v>286</v>
       </c>
@@ -6661,40 +6684,40 @@
       <c r="P14" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="Q14" s="34" t="s">
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34" t="s">
         <v>372</v>
       </c>
-      <c r="R14" s="34" t="s">
+      <c r="S14" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="S14" s="34" t="s">
-        <v>34</v>
-      </c>
       <c r="T14" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="U14" s="34" t="s">
         <v>374</v>
       </c>
-      <c r="U14" s="34" t="s">
+      <c r="V14" s="34" t="s">
         <v>375</v>
       </c>
-      <c r="V14" s="34" t="s">
+      <c r="W14" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="W14" s="48">
+      <c r="X14" s="48">
         <v>1000</v>
       </c>
-      <c r="X14" s="34">
+      <c r="Y14" s="34">
         <v>1000</v>
-      </c>
-      <c r="Y14" s="34">
-        <v>500</v>
       </c>
       <c r="Z14" s="34">
         <v>500</v>
       </c>
-      <c r="AA14" s="38"/>
+      <c r="AA14" s="34">
+        <v>500</v>
+      </c>
       <c r="AB14" s="38"/>
-      <c r="AC14" s="20"/>
-      <c r="AD14" s="35"/>
+      <c r="AC14" s="38"/>
+      <c r="AD14" s="20"/>
       <c r="AE14" s="35"/>
       <c r="AF14" s="35"/>
       <c r="AG14" s="35"/>
@@ -6703,23 +6726,24 @@
       <c r="AJ14" s="35"/>
       <c r="AK14" s="35"/>
       <c r="AL14" s="35"/>
-      <c r="AM14" s="35"/>
-      <c r="AN14" s="35"/>
+      <c r="AM14" s="49"/>
+      <c r="AN14" s="49"/>
       <c r="AO14" s="35"/>
       <c r="AP14" s="35"/>
       <c r="AQ14" s="35"/>
       <c r="AR14" s="35"/>
       <c r="AS14" s="35"/>
-      <c r="AT14" s="20"/>
+      <c r="AT14" s="35"/>
       <c r="AU14" s="20"/>
       <c r="AV14" s="20"/>
       <c r="AW14" s="20"/>
       <c r="AX14" s="20"/>
-      <c r="AY14" s="20"/>
-      <c r="AZ14" s="20"/>
+      <c r="AY14" s="27"/>
+      <c r="AZ14" s="27"/>
       <c r="BA14" s="20"/>
-    </row>
-    <row r="15" spans="1:65" ht="15.75">
+      <c r="BB14" s="20"/>
+    </row>
+    <row r="15" spans="1:66" ht="15.75">
       <c r="A15" s="20" t="s">
         <v>288</v>
       </c>
@@ -6744,22 +6768,22 @@
       <c r="N15" s="34"/>
       <c r="O15" s="34"/>
       <c r="P15" s="34"/>
-      <c r="Q15" s="9"/>
+      <c r="Q15" s="34"/>
       <c r="R15" s="9"/>
-      <c r="S15" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U15" s="9"/>
       <c r="V15" s="9"/>
       <c r="W15" s="9"/>
       <c r="X15" s="9"/>
       <c r="Y15" s="9"/>
       <c r="Z15" s="9"/>
-      <c r="AA15" s="38"/>
+      <c r="AA15" s="9"/>
       <c r="AB15" s="38"/>
-      <c r="AC15" s="20"/>
-      <c r="AD15" s="35"/>
+      <c r="AC15" s="38"/>
+      <c r="AD15" s="20"/>
       <c r="AE15" s="35"/>
       <c r="AF15" s="35"/>
       <c r="AG15" s="35"/>
@@ -6768,23 +6792,24 @@
       <c r="AJ15" s="35"/>
       <c r="AK15" s="35"/>
       <c r="AL15" s="35"/>
-      <c r="AM15" s="35"/>
-      <c r="AN15" s="35"/>
+      <c r="AM15" s="49"/>
+      <c r="AN15" s="49"/>
       <c r="AO15" s="35"/>
       <c r="AP15" s="35"/>
       <c r="AQ15" s="35"/>
       <c r="AR15" s="35"/>
       <c r="AS15" s="35"/>
-      <c r="AT15" s="20"/>
+      <c r="AT15" s="35"/>
       <c r="AU15" s="20"/>
       <c r="AV15" s="20"/>
       <c r="AW15" s="20"/>
       <c r="AX15" s="20"/>
-      <c r="AY15" s="20"/>
-      <c r="AZ15" s="20"/>
+      <c r="AY15" s="27"/>
+      <c r="AZ15" s="27"/>
       <c r="BA15" s="20"/>
-    </row>
-    <row r="16" spans="1:65" ht="15.75">
+      <c r="BB15" s="20"/>
+    </row>
+    <row r="16" spans="1:66" ht="15.75">
       <c r="A16" s="20" t="s">
         <v>289</v>
       </c>
@@ -6805,22 +6830,22 @@
       <c r="N16" s="34"/>
       <c r="O16" s="34"/>
       <c r="P16" s="34"/>
-      <c r="Q16" s="9"/>
+      <c r="Q16" s="34"/>
       <c r="R16" s="9"/>
-      <c r="S16" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U16" s="9"/>
       <c r="V16" s="9"/>
       <c r="W16" s="9"/>
       <c r="X16" s="9"/>
       <c r="Y16" s="9"/>
       <c r="Z16" s="9"/>
-      <c r="AA16" s="38"/>
+      <c r="AA16" s="9"/>
       <c r="AB16" s="38"/>
-      <c r="AC16" s="20"/>
-      <c r="AD16" s="35"/>
+      <c r="AC16" s="38"/>
+      <c r="AD16" s="20"/>
       <c r="AE16" s="35"/>
       <c r="AF16" s="35"/>
       <c r="AG16" s="35"/>
@@ -6829,23 +6854,24 @@
       <c r="AJ16" s="35"/>
       <c r="AK16" s="35"/>
       <c r="AL16" s="35"/>
-      <c r="AM16" s="35"/>
-      <c r="AN16" s="35"/>
+      <c r="AM16" s="49"/>
+      <c r="AN16" s="49"/>
       <c r="AO16" s="35"/>
       <c r="AP16" s="35"/>
       <c r="AQ16" s="35"/>
       <c r="AR16" s="35"/>
       <c r="AS16" s="35"/>
-      <c r="AT16" s="20"/>
+      <c r="AT16" s="35"/>
       <c r="AU16" s="20"/>
       <c r="AV16" s="20"/>
       <c r="AW16" s="20"/>
       <c r="AX16" s="20"/>
-      <c r="AY16" s="20"/>
-      <c r="AZ16" s="20"/>
+      <c r="AY16" s="27"/>
+      <c r="AZ16" s="27"/>
       <c r="BA16" s="20"/>
-    </row>
-    <row r="17" spans="1:53" ht="15.75">
+      <c r="BB16" s="20"/>
+    </row>
+    <row r="17" spans="1:54" ht="15.75">
       <c r="A17" s="20" t="s">
         <v>290</v>
       </c>
@@ -6866,22 +6892,22 @@
       <c r="N17" s="34"/>
       <c r="O17" s="34"/>
       <c r="P17" s="34"/>
-      <c r="Q17" s="9"/>
+      <c r="Q17" s="34"/>
       <c r="R17" s="9"/>
-      <c r="S17" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U17" s="9"/>
       <c r="V17" s="9"/>
       <c r="W17" s="9"/>
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
       <c r="Z17" s="9"/>
-      <c r="AA17" s="38"/>
+      <c r="AA17" s="9"/>
       <c r="AB17" s="38"/>
-      <c r="AC17" s="20"/>
-      <c r="AD17" s="35"/>
+      <c r="AC17" s="38"/>
+      <c r="AD17" s="20"/>
       <c r="AE17" s="35"/>
       <c r="AF17" s="35"/>
       <c r="AG17" s="35"/>
@@ -6890,23 +6916,24 @@
       <c r="AJ17" s="35"/>
       <c r="AK17" s="35"/>
       <c r="AL17" s="35"/>
-      <c r="AM17" s="35"/>
-      <c r="AN17" s="35"/>
+      <c r="AM17" s="49"/>
+      <c r="AN17" s="49"/>
       <c r="AO17" s="35"/>
       <c r="AP17" s="35"/>
       <c r="AQ17" s="35"/>
       <c r="AR17" s="35"/>
       <c r="AS17" s="35"/>
-      <c r="AT17" s="20"/>
+      <c r="AT17" s="35"/>
       <c r="AU17" s="20"/>
       <c r="AV17" s="20"/>
       <c r="AW17" s="20"/>
       <c r="AX17" s="20"/>
-      <c r="AY17" s="20"/>
-      <c r="AZ17" s="20"/>
+      <c r="AY17" s="27"/>
+      <c r="AZ17" s="27"/>
       <c r="BA17" s="20"/>
-    </row>
-    <row r="18" spans="1:53" ht="15.75">
+      <c r="BB17" s="20"/>
+    </row>
+    <row r="18" spans="1:54" ht="15.75">
       <c r="A18" s="20" t="s">
         <v>294</v>
       </c>
@@ -6929,40 +6956,40 @@
       <c r="P18" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="Q18" s="34" t="s">
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34" t="s">
         <v>372</v>
       </c>
-      <c r="R18" s="34" t="s">
+      <c r="S18" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="S18" s="34" t="s">
-        <v>34</v>
-      </c>
       <c r="T18" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="U18" s="34" t="s">
         <v>374</v>
       </c>
-      <c r="U18" s="34" t="s">
+      <c r="V18" s="34" t="s">
         <v>375</v>
       </c>
-      <c r="V18" s="34" t="s">
+      <c r="W18" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="W18" s="48">
+      <c r="X18" s="48">
         <v>1000</v>
       </c>
-      <c r="X18" s="34">
+      <c r="Y18" s="34">
         <v>1000</v>
-      </c>
-      <c r="Y18" s="34">
-        <v>500</v>
       </c>
       <c r="Z18" s="34">
         <v>500</v>
       </c>
-      <c r="AA18" s="38"/>
+      <c r="AA18" s="34">
+        <v>500</v>
+      </c>
       <c r="AB18" s="38"/>
-      <c r="AC18" s="20"/>
-      <c r="AD18" s="35"/>
+      <c r="AC18" s="38"/>
+      <c r="AD18" s="20"/>
       <c r="AE18" s="35"/>
       <c r="AF18" s="35"/>
       <c r="AG18" s="35"/>
@@ -6971,23 +6998,24 @@
       <c r="AJ18" s="35"/>
       <c r="AK18" s="35"/>
       <c r="AL18" s="35"/>
-      <c r="AM18" s="35"/>
-      <c r="AN18" s="35"/>
+      <c r="AM18" s="49"/>
+      <c r="AN18" s="49"/>
       <c r="AO18" s="35"/>
       <c r="AP18" s="35"/>
       <c r="AQ18" s="35"/>
       <c r="AR18" s="35"/>
       <c r="AS18" s="35"/>
-      <c r="AT18" s="20"/>
+      <c r="AT18" s="35"/>
       <c r="AU18" s="20"/>
       <c r="AV18" s="20"/>
       <c r="AW18" s="20"/>
       <c r="AX18" s="20"/>
-      <c r="AY18" s="20"/>
-      <c r="AZ18" s="20"/>
+      <c r="AY18" s="27"/>
+      <c r="AZ18" s="27"/>
       <c r="BA18" s="20"/>
-    </row>
-    <row r="19" spans="1:53" ht="15.75">
+      <c r="BB18" s="20"/>
+    </row>
+    <row r="19" spans="1:54" ht="15.75">
       <c r="A19" s="20" t="s">
         <v>295</v>
       </c>
@@ -7012,22 +7040,22 @@
       <c r="N19" s="34"/>
       <c r="O19" s="34"/>
       <c r="P19" s="34"/>
-      <c r="Q19" s="9"/>
+      <c r="Q19" s="34"/>
       <c r="R19" s="9"/>
-      <c r="S19" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U19" s="9"/>
       <c r="V19" s="9"/>
       <c r="W19" s="9"/>
       <c r="X19" s="9"/>
       <c r="Y19" s="9"/>
       <c r="Z19" s="9"/>
-      <c r="AA19" s="38"/>
+      <c r="AA19" s="9"/>
       <c r="AB19" s="38"/>
-      <c r="AC19" s="20"/>
-      <c r="AD19" s="35"/>
+      <c r="AC19" s="38"/>
+      <c r="AD19" s="20"/>
       <c r="AE19" s="35"/>
       <c r="AF19" s="35"/>
       <c r="AG19" s="35"/>
@@ -7036,23 +7064,24 @@
       <c r="AJ19" s="35"/>
       <c r="AK19" s="35"/>
       <c r="AL19" s="35"/>
-      <c r="AM19" s="35"/>
-      <c r="AN19" s="35"/>
+      <c r="AM19" s="49"/>
+      <c r="AN19" s="49"/>
       <c r="AO19" s="35"/>
       <c r="AP19" s="35"/>
       <c r="AQ19" s="35"/>
       <c r="AR19" s="35"/>
       <c r="AS19" s="35"/>
-      <c r="AT19" s="20"/>
+      <c r="AT19" s="35"/>
       <c r="AU19" s="20"/>
       <c r="AV19" s="20"/>
       <c r="AW19" s="20"/>
       <c r="AX19" s="20"/>
-      <c r="AY19" s="20"/>
-      <c r="AZ19" s="20"/>
+      <c r="AY19" s="27"/>
+      <c r="AZ19" s="27"/>
       <c r="BA19" s="20"/>
-    </row>
-    <row r="20" spans="1:53" ht="15.75">
+      <c r="BB19" s="20"/>
+    </row>
+    <row r="20" spans="1:54" ht="15.75">
       <c r="A20" s="20" t="s">
         <v>296</v>
       </c>
@@ -7073,22 +7102,22 @@
       <c r="N20" s="34"/>
       <c r="O20" s="34"/>
       <c r="P20" s="34"/>
-      <c r="Q20" s="9"/>
+      <c r="Q20" s="34"/>
       <c r="R20" s="9"/>
-      <c r="S20" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U20" s="9"/>
       <c r="V20" s="9"/>
       <c r="W20" s="9"/>
       <c r="X20" s="9"/>
       <c r="Y20" s="9"/>
       <c r="Z20" s="9"/>
-      <c r="AA20" s="38"/>
+      <c r="AA20" s="9"/>
       <c r="AB20" s="38"/>
-      <c r="AC20" s="20"/>
-      <c r="AD20" s="35"/>
+      <c r="AC20" s="38"/>
+      <c r="AD20" s="20"/>
       <c r="AE20" s="35"/>
       <c r="AF20" s="35"/>
       <c r="AG20" s="35"/>
@@ -7097,23 +7126,24 @@
       <c r="AJ20" s="35"/>
       <c r="AK20" s="35"/>
       <c r="AL20" s="35"/>
-      <c r="AM20" s="35"/>
-      <c r="AN20" s="35"/>
+      <c r="AM20" s="49"/>
+      <c r="AN20" s="49"/>
       <c r="AO20" s="35"/>
       <c r="AP20" s="35"/>
       <c r="AQ20" s="35"/>
       <c r="AR20" s="35"/>
       <c r="AS20" s="35"/>
-      <c r="AT20" s="20"/>
+      <c r="AT20" s="35"/>
       <c r="AU20" s="20"/>
       <c r="AV20" s="20"/>
       <c r="AW20" s="20"/>
       <c r="AX20" s="20"/>
-      <c r="AY20" s="20"/>
-      <c r="AZ20" s="20"/>
+      <c r="AY20" s="27"/>
+      <c r="AZ20" s="27"/>
       <c r="BA20" s="20"/>
-    </row>
-    <row r="21" spans="1:53" ht="15.75">
+      <c r="BB20" s="20"/>
+    </row>
+    <row r="21" spans="1:54" ht="15.75">
       <c r="A21" s="20" t="s">
         <v>297</v>
       </c>
@@ -7134,22 +7164,22 @@
       <c r="N21" s="34"/>
       <c r="O21" s="34"/>
       <c r="P21" s="34"/>
-      <c r="Q21" s="9"/>
+      <c r="Q21" s="34"/>
       <c r="R21" s="9"/>
-      <c r="S21" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U21" s="9"/>
       <c r="V21" s="9"/>
       <c r="W21" s="9"/>
       <c r="X21" s="9"/>
       <c r="Y21" s="9"/>
       <c r="Z21" s="9"/>
-      <c r="AA21" s="38"/>
+      <c r="AA21" s="9"/>
       <c r="AB21" s="38"/>
-      <c r="AC21" s="20"/>
-      <c r="AD21" s="35"/>
+      <c r="AC21" s="38"/>
+      <c r="AD21" s="20"/>
       <c r="AE21" s="35"/>
       <c r="AF21" s="35"/>
       <c r="AG21" s="35"/>
@@ -7158,23 +7188,24 @@
       <c r="AJ21" s="35"/>
       <c r="AK21" s="35"/>
       <c r="AL21" s="35"/>
-      <c r="AM21" s="35"/>
-      <c r="AN21" s="35"/>
+      <c r="AM21" s="49"/>
+      <c r="AN21" s="49"/>
       <c r="AO21" s="35"/>
       <c r="AP21" s="35"/>
       <c r="AQ21" s="35"/>
       <c r="AR21" s="35"/>
       <c r="AS21" s="35"/>
-      <c r="AT21" s="20"/>
+      <c r="AT21" s="35"/>
       <c r="AU21" s="20"/>
       <c r="AV21" s="20"/>
       <c r="AW21" s="20"/>
       <c r="AX21" s="20"/>
-      <c r="AY21" s="20"/>
-      <c r="AZ21" s="20"/>
+      <c r="AY21" s="27"/>
+      <c r="AZ21" s="27"/>
       <c r="BA21" s="20"/>
-    </row>
-    <row r="22" spans="1:53" ht="15.75">
+      <c r="BB21" s="20"/>
+    </row>
+    <row r="22" spans="1:54" ht="15.75">
       <c r="A22" s="20" t="s">
         <v>302</v>
       </c>
@@ -7197,24 +7228,24 @@
       <c r="P22" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="Q22" s="9"/>
+      <c r="Q22" s="34"/>
       <c r="R22" s="9"/>
-      <c r="S22" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U22" s="9"/>
       <c r="V22" s="9"/>
       <c r="W22" s="9"/>
       <c r="X22" s="9"/>
       <c r="Y22" s="9"/>
       <c r="Z22" s="9"/>
-      <c r="AA22" s="38" t="s">
+      <c r="AA22" s="9"/>
+      <c r="AB22" s="38" t="s">
         <v>438</v>
       </c>
-      <c r="AB22" s="38"/>
-      <c r="AC22" s="20"/>
-      <c r="AD22" s="35"/>
+      <c r="AC22" s="38"/>
+      <c r="AD22" s="20"/>
       <c r="AE22" s="35"/>
       <c r="AF22" s="35"/>
       <c r="AG22" s="35"/>
@@ -7223,23 +7254,24 @@
       <c r="AJ22" s="35"/>
       <c r="AK22" s="35"/>
       <c r="AL22" s="35"/>
-      <c r="AM22" s="35"/>
-      <c r="AN22" s="35"/>
+      <c r="AM22" s="49"/>
+      <c r="AN22" s="49"/>
       <c r="AO22" s="35"/>
       <c r="AP22" s="35"/>
       <c r="AQ22" s="35"/>
       <c r="AR22" s="35"/>
       <c r="AS22" s="35"/>
-      <c r="AT22" s="20"/>
+      <c r="AT22" s="35"/>
       <c r="AU22" s="20"/>
       <c r="AV22" s="20"/>
       <c r="AW22" s="20"/>
       <c r="AX22" s="20"/>
-      <c r="AY22" s="20"/>
-      <c r="AZ22" s="20"/>
+      <c r="AY22" s="27"/>
+      <c r="AZ22" s="27"/>
       <c r="BA22" s="20"/>
-    </row>
-    <row r="23" spans="1:53" ht="15.75">
+      <c r="BB22" s="20"/>
+    </row>
+    <row r="23" spans="1:54" ht="15.75">
       <c r="A23" s="20" t="s">
         <v>303</v>
       </c>
@@ -7260,24 +7292,24 @@
       <c r="N23" s="34"/>
       <c r="O23" s="34"/>
       <c r="P23" s="34"/>
-      <c r="Q23" s="9"/>
+      <c r="Q23" s="34"/>
       <c r="R23" s="9"/>
-      <c r="S23" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U23" s="9"/>
       <c r="V23" s="9"/>
       <c r="W23" s="9"/>
       <c r="X23" s="9"/>
       <c r="Y23" s="9"/>
       <c r="Z23" s="9"/>
-      <c r="AA23" s="38"/>
+      <c r="AA23" s="9"/>
       <c r="AB23" s="38"/>
-      <c r="AC23" s="20" t="s">
+      <c r="AC23" s="38"/>
+      <c r="AD23" s="20" t="s">
         <v>408</v>
       </c>
-      <c r="AD23" s="35"/>
       <c r="AE23" s="35"/>
       <c r="AF23" s="35"/>
       <c r="AG23" s="35"/>
@@ -7286,23 +7318,24 @@
       <c r="AJ23" s="35"/>
       <c r="AK23" s="35"/>
       <c r="AL23" s="35"/>
-      <c r="AM23" s="35"/>
-      <c r="AN23" s="35"/>
+      <c r="AM23" s="49"/>
+      <c r="AN23" s="49"/>
       <c r="AO23" s="35"/>
       <c r="AP23" s="35"/>
       <c r="AQ23" s="35"/>
       <c r="AR23" s="35"/>
       <c r="AS23" s="35"/>
-      <c r="AT23" s="20"/>
+      <c r="AT23" s="35"/>
       <c r="AU23" s="20"/>
       <c r="AV23" s="20"/>
       <c r="AW23" s="20"/>
       <c r="AX23" s="20"/>
-      <c r="AY23" s="20"/>
-      <c r="AZ23" s="20"/>
+      <c r="AY23" s="27"/>
+      <c r="AZ23" s="27"/>
       <c r="BA23" s="20"/>
-    </row>
-    <row r="24" spans="1:53" ht="15.75">
+      <c r="BB23" s="20"/>
+    </row>
+    <row r="24" spans="1:54" ht="15.75">
       <c r="A24" s="20" t="s">
         <v>304</v>
       </c>
@@ -7327,22 +7360,22 @@
       <c r="N24" s="34"/>
       <c r="O24" s="34"/>
       <c r="P24" s="34"/>
-      <c r="Q24" s="9"/>
+      <c r="Q24" s="34"/>
       <c r="R24" s="9"/>
-      <c r="S24" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U24" s="9"/>
       <c r="V24" s="9"/>
       <c r="W24" s="9"/>
       <c r="X24" s="9"/>
       <c r="Y24" s="9"/>
       <c r="Z24" s="9"/>
-      <c r="AA24" s="38"/>
+      <c r="AA24" s="9"/>
       <c r="AB24" s="38"/>
-      <c r="AC24" s="20"/>
-      <c r="AD24" s="35"/>
+      <c r="AC24" s="38"/>
+      <c r="AD24" s="20"/>
       <c r="AE24" s="35"/>
       <c r="AF24" s="35"/>
       <c r="AG24" s="35"/>
@@ -7351,23 +7384,24 @@
       <c r="AJ24" s="35"/>
       <c r="AK24" s="35"/>
       <c r="AL24" s="35"/>
-      <c r="AM24" s="35"/>
-      <c r="AN24" s="35"/>
+      <c r="AM24" s="49"/>
+      <c r="AN24" s="49"/>
       <c r="AO24" s="35"/>
       <c r="AP24" s="35"/>
       <c r="AQ24" s="35"/>
       <c r="AR24" s="35"/>
       <c r="AS24" s="35"/>
-      <c r="AT24" s="20"/>
+      <c r="AT24" s="35"/>
       <c r="AU24" s="20"/>
       <c r="AV24" s="20"/>
       <c r="AW24" s="20"/>
       <c r="AX24" s="20"/>
-      <c r="AY24" s="20"/>
-      <c r="AZ24" s="20"/>
+      <c r="AY24" s="27"/>
+      <c r="AZ24" s="27"/>
       <c r="BA24" s="20"/>
-    </row>
-    <row r="25" spans="1:53" ht="15.75">
+      <c r="BB24" s="20"/>
+    </row>
+    <row r="25" spans="1:54" ht="15.75">
       <c r="A25" s="20" t="s">
         <v>305</v>
       </c>
@@ -7388,22 +7422,22 @@
       <c r="N25" s="34"/>
       <c r="O25" s="34"/>
       <c r="P25" s="34"/>
-      <c r="Q25" s="9"/>
+      <c r="Q25" s="34"/>
       <c r="R25" s="9"/>
-      <c r="S25" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U25" s="9"/>
       <c r="V25" s="9"/>
       <c r="W25" s="9"/>
       <c r="X25" s="9"/>
       <c r="Y25" s="9"/>
       <c r="Z25" s="9"/>
-      <c r="AA25" s="38"/>
+      <c r="AA25" s="9"/>
       <c r="AB25" s="38"/>
-      <c r="AC25" s="20"/>
-      <c r="AD25" s="35"/>
+      <c r="AC25" s="38"/>
+      <c r="AD25" s="20"/>
       <c r="AE25" s="35"/>
       <c r="AF25" s="35"/>
       <c r="AG25" s="35"/>
@@ -7412,23 +7446,24 @@
       <c r="AJ25" s="35"/>
       <c r="AK25" s="35"/>
       <c r="AL25" s="35"/>
-      <c r="AM25" s="35"/>
-      <c r="AN25" s="35"/>
+      <c r="AM25" s="49"/>
+      <c r="AN25" s="49"/>
       <c r="AO25" s="35"/>
       <c r="AP25" s="35"/>
       <c r="AQ25" s="35"/>
       <c r="AR25" s="35"/>
       <c r="AS25" s="35"/>
-      <c r="AT25" s="20"/>
+      <c r="AT25" s="35"/>
       <c r="AU25" s="20"/>
       <c r="AV25" s="20"/>
       <c r="AW25" s="20"/>
       <c r="AX25" s="20"/>
-      <c r="AY25" s="20"/>
-      <c r="AZ25" s="20"/>
+      <c r="AY25" s="27"/>
+      <c r="AZ25" s="27"/>
       <c r="BA25" s="20"/>
-    </row>
-    <row r="26" spans="1:53" ht="15.75">
+      <c r="BB25" s="20"/>
+    </row>
+    <row r="26" spans="1:54" ht="15.75">
       <c r="A26" s="20" t="s">
         <v>306</v>
       </c>
@@ -7449,24 +7484,24 @@
       <c r="N26" s="34"/>
       <c r="O26" s="34"/>
       <c r="P26" s="34"/>
-      <c r="Q26" s="9"/>
+      <c r="Q26" s="34"/>
       <c r="R26" s="9"/>
-      <c r="S26" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U26" s="9"/>
       <c r="V26" s="9"/>
       <c r="W26" s="9"/>
       <c r="X26" s="9"/>
       <c r="Y26" s="9"/>
       <c r="Z26" s="9"/>
-      <c r="AA26" s="38" t="s">
+      <c r="AA26" s="9"/>
+      <c r="AB26" s="38" t="s">
         <v>438</v>
       </c>
-      <c r="AB26" s="38"/>
-      <c r="AC26" s="20"/>
-      <c r="AD26" s="35"/>
+      <c r="AC26" s="38"/>
+      <c r="AD26" s="20"/>
       <c r="AE26" s="35"/>
       <c r="AF26" s="35"/>
       <c r="AG26" s="35"/>
@@ -7475,23 +7510,24 @@
       <c r="AJ26" s="35"/>
       <c r="AK26" s="35"/>
       <c r="AL26" s="35"/>
-      <c r="AM26" s="35"/>
-      <c r="AN26" s="35"/>
+      <c r="AM26" s="49"/>
+      <c r="AN26" s="49"/>
       <c r="AO26" s="35"/>
       <c r="AP26" s="35"/>
       <c r="AQ26" s="35"/>
       <c r="AR26" s="35"/>
       <c r="AS26" s="35"/>
-      <c r="AT26" s="20"/>
+      <c r="AT26" s="35"/>
       <c r="AU26" s="20"/>
       <c r="AV26" s="20"/>
       <c r="AW26" s="20"/>
       <c r="AX26" s="20"/>
-      <c r="AY26" s="20"/>
-      <c r="AZ26" s="20"/>
+      <c r="AY26" s="27"/>
+      <c r="AZ26" s="27"/>
       <c r="BA26" s="20"/>
-    </row>
-    <row r="27" spans="1:53" ht="15.75">
+      <c r="BB26" s="20"/>
+    </row>
+    <row r="27" spans="1:54" ht="15.75">
       <c r="A27" s="20" t="s">
         <v>311</v>
       </c>
@@ -7512,24 +7548,24 @@
       <c r="N27" s="34"/>
       <c r="O27" s="34"/>
       <c r="P27" s="34"/>
-      <c r="Q27" s="9"/>
+      <c r="Q27" s="34"/>
       <c r="R27" s="9"/>
-      <c r="S27" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U27" s="9"/>
       <c r="V27" s="9"/>
       <c r="W27" s="9"/>
       <c r="X27" s="9"/>
       <c r="Y27" s="9"/>
       <c r="Z27" s="9"/>
-      <c r="AA27" s="38" t="s">
+      <c r="AA27" s="9"/>
+      <c r="AB27" s="38" t="s">
         <v>438</v>
       </c>
-      <c r="AB27" s="38"/>
-      <c r="AC27" s="20"/>
-      <c r="AD27" s="35"/>
+      <c r="AC27" s="38"/>
+      <c r="AD27" s="20"/>
       <c r="AE27" s="35"/>
       <c r="AF27" s="35"/>
       <c r="AG27" s="35"/>
@@ -7538,23 +7574,24 @@
       <c r="AJ27" s="35"/>
       <c r="AK27" s="35"/>
       <c r="AL27" s="35"/>
-      <c r="AM27" s="35"/>
-      <c r="AN27" s="35"/>
+      <c r="AM27" s="49"/>
+      <c r="AN27" s="49"/>
       <c r="AO27" s="35"/>
       <c r="AP27" s="35"/>
       <c r="AQ27" s="35"/>
       <c r="AR27" s="35"/>
       <c r="AS27" s="35"/>
-      <c r="AT27" s="20"/>
+      <c r="AT27" s="35"/>
       <c r="AU27" s="20"/>
       <c r="AV27" s="20"/>
       <c r="AW27" s="20"/>
       <c r="AX27" s="20"/>
-      <c r="AY27" s="20"/>
-      <c r="AZ27" s="20"/>
+      <c r="AY27" s="27"/>
+      <c r="AZ27" s="27"/>
       <c r="BA27" s="20"/>
-    </row>
-    <row r="28" spans="1:53" ht="15.75">
+      <c r="BB27" s="20"/>
+    </row>
+    <row r="28" spans="1:54" ht="15.75">
       <c r="A28" s="20" t="s">
         <v>314</v>
       </c>
@@ -7575,63 +7612,64 @@
       <c r="N28" s="34"/>
       <c r="O28" s="34"/>
       <c r="P28" s="34"/>
-      <c r="Q28" s="9"/>
+      <c r="Q28" s="34"/>
       <c r="R28" s="9"/>
-      <c r="S28" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U28" s="9"/>
       <c r="V28" s="9"/>
       <c r="W28" s="9"/>
       <c r="X28" s="9"/>
       <c r="Y28" s="9"/>
       <c r="Z28" s="9"/>
-      <c r="AA28" s="38"/>
+      <c r="AA28" s="9"/>
       <c r="AB28" s="38"/>
-      <c r="AC28" s="20"/>
-      <c r="AD28" s="29" t="s">
+      <c r="AC28" s="38"/>
+      <c r="AD28" s="20"/>
+      <c r="AE28" s="29" t="s">
         <v>360</v>
       </c>
-      <c r="AE28" s="29" t="s">
+      <c r="AF28" s="29" t="s">
         <v>416</v>
       </c>
-      <c r="AF28" s="29" t="s">
+      <c r="AG28" s="29" t="s">
         <v>417</v>
       </c>
-      <c r="AG28" s="35">
+      <c r="AH28" s="35">
         <v>6</v>
       </c>
-      <c r="AH28" s="35" t="s">
+      <c r="AI28" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="AI28" s="35" t="s">
+      <c r="AJ28" s="35" t="s">
         <v>418</v>
       </c>
-      <c r="AJ28" s="35">
+      <c r="AK28" s="35">
         <v>2022</v>
       </c>
-      <c r="AK28" s="35" t="s">
+      <c r="AL28" s="35" t="s">
         <v>372</v>
       </c>
-      <c r="AL28" s="35"/>
-      <c r="AM28" s="35"/>
-      <c r="AN28" s="35"/>
+      <c r="AM28" s="49"/>
+      <c r="AN28" s="49"/>
       <c r="AO28" s="35"/>
       <c r="AP28" s="35"/>
       <c r="AQ28" s="35"/>
       <c r="AR28" s="35"/>
       <c r="AS28" s="35"/>
-      <c r="AT28" s="20"/>
+      <c r="AT28" s="35"/>
       <c r="AU28" s="20"/>
       <c r="AV28" s="20"/>
       <c r="AW28" s="20"/>
       <c r="AX28" s="20"/>
-      <c r="AY28" s="20"/>
-      <c r="AZ28" s="20"/>
+      <c r="AY28" s="27"/>
+      <c r="AZ28" s="27"/>
       <c r="BA28" s="20"/>
-    </row>
-    <row r="29" spans="1:53" ht="15.75">
+      <c r="BB28" s="20"/>
+    </row>
+    <row r="29" spans="1:54" ht="15.75">
       <c r="A29" s="20" t="s">
         <v>314</v>
       </c>
@@ -7652,63 +7690,64 @@
       <c r="N29" s="34"/>
       <c r="O29" s="34"/>
       <c r="P29" s="34"/>
-      <c r="Q29" s="9"/>
+      <c r="Q29" s="34"/>
       <c r="R29" s="9"/>
-      <c r="S29" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U29" s="9"/>
       <c r="V29" s="9"/>
       <c r="W29" s="9"/>
       <c r="X29" s="9"/>
       <c r="Y29" s="9"/>
       <c r="Z29" s="9"/>
-      <c r="AA29" s="38"/>
+      <c r="AA29" s="9"/>
       <c r="AB29" s="38"/>
-      <c r="AC29" s="20"/>
-      <c r="AD29" s="29" t="s">
+      <c r="AC29" s="38"/>
+      <c r="AD29" s="20"/>
+      <c r="AE29" s="29" t="s">
         <v>422</v>
       </c>
-      <c r="AE29" s="29" t="s">
+      <c r="AF29" s="29" t="s">
         <v>423</v>
       </c>
-      <c r="AF29" s="29" t="s">
+      <c r="AG29" s="29" t="s">
         <v>282</v>
       </c>
-      <c r="AG29" s="35">
+      <c r="AH29" s="35">
         <v>7</v>
       </c>
-      <c r="AH29" s="35" t="s">
+      <c r="AI29" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="AI29" s="35" t="s">
+      <c r="AJ29" s="35" t="s">
         <v>418</v>
       </c>
-      <c r="AJ29" s="35">
+      <c r="AK29" s="35">
         <v>2022</v>
       </c>
-      <c r="AK29" s="35" t="s">
+      <c r="AL29" s="35" t="s">
         <v>372</v>
       </c>
-      <c r="AL29" s="35"/>
-      <c r="AM29" s="35"/>
-      <c r="AN29" s="35"/>
+      <c r="AM29" s="49"/>
+      <c r="AN29" s="49"/>
       <c r="AO29" s="35"/>
       <c r="AP29" s="35"/>
       <c r="AQ29" s="35"/>
       <c r="AR29" s="35"/>
       <c r="AS29" s="35"/>
-      <c r="AT29" s="20"/>
+      <c r="AT29" s="35"/>
       <c r="AU29" s="20"/>
       <c r="AV29" s="20"/>
       <c r="AW29" s="20"/>
       <c r="AX29" s="20"/>
-      <c r="AY29" s="20"/>
-      <c r="AZ29" s="20"/>
+      <c r="AY29" s="27"/>
+      <c r="AZ29" s="27"/>
       <c r="BA29" s="20"/>
-    </row>
-    <row r="30" spans="1:53" ht="15.75">
+      <c r="BB29" s="20"/>
+    </row>
+    <row r="30" spans="1:54" ht="15.75">
       <c r="A30" s="20" t="s">
         <v>314</v>
       </c>
@@ -7729,63 +7768,64 @@
       <c r="N30" s="34"/>
       <c r="O30" s="34"/>
       <c r="P30" s="34"/>
-      <c r="Q30" s="9"/>
+      <c r="Q30" s="34"/>
       <c r="R30" s="9"/>
-      <c r="S30" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U30" s="9"/>
       <c r="V30" s="9"/>
       <c r="W30" s="9"/>
       <c r="X30" s="9"/>
       <c r="Y30" s="9"/>
       <c r="Z30" s="9"/>
-      <c r="AA30" s="38"/>
+      <c r="AA30" s="9"/>
       <c r="AB30" s="38"/>
-      <c r="AC30" s="20"/>
-      <c r="AD30" s="29" t="s">
+      <c r="AC30" s="38"/>
+      <c r="AD30" s="20"/>
+      <c r="AE30" s="29" t="s">
         <v>424</v>
       </c>
-      <c r="AE30" s="29" t="s">
+      <c r="AF30" s="29" t="s">
         <v>416</v>
       </c>
-      <c r="AF30" s="29" t="s">
+      <c r="AG30" s="29" t="s">
         <v>425</v>
       </c>
-      <c r="AG30" s="35">
+      <c r="AH30" s="35">
         <v>8</v>
       </c>
-      <c r="AH30" s="35" t="s">
+      <c r="AI30" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="AI30" s="35" t="s">
+      <c r="AJ30" s="35" t="s">
         <v>418</v>
       </c>
-      <c r="AJ30" s="35">
+      <c r="AK30" s="35">
         <v>2022</v>
       </c>
-      <c r="AK30" s="35" t="s">
+      <c r="AL30" s="35" t="s">
         <v>372</v>
       </c>
-      <c r="AL30" s="35"/>
-      <c r="AM30" s="35"/>
-      <c r="AN30" s="35"/>
+      <c r="AM30" s="49"/>
+      <c r="AN30" s="49"/>
       <c r="AO30" s="35"/>
       <c r="AP30" s="35"/>
       <c r="AQ30" s="35"/>
       <c r="AR30" s="35"/>
       <c r="AS30" s="35"/>
-      <c r="AT30" s="20"/>
+      <c r="AT30" s="35"/>
       <c r="AU30" s="20"/>
       <c r="AV30" s="20"/>
       <c r="AW30" s="20"/>
       <c r="AX30" s="20"/>
-      <c r="AY30" s="20"/>
-      <c r="AZ30" s="20"/>
+      <c r="AY30" s="27"/>
+      <c r="AZ30" s="27"/>
       <c r="BA30" s="20"/>
-    </row>
-    <row r="31" spans="1:53" ht="15.75">
+      <c r="BB30" s="20"/>
+    </row>
+    <row r="31" spans="1:54" ht="15.75">
       <c r="A31" s="20" t="s">
         <v>314</v>
       </c>
@@ -7806,63 +7846,64 @@
       <c r="N31" s="34"/>
       <c r="O31" s="34"/>
       <c r="P31" s="34"/>
-      <c r="Q31" s="9"/>
+      <c r="Q31" s="34"/>
       <c r="R31" s="9"/>
-      <c r="S31" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U31" s="9"/>
       <c r="V31" s="9"/>
       <c r="W31" s="9"/>
       <c r="X31" s="9"/>
       <c r="Y31" s="9"/>
       <c r="Z31" s="9"/>
-      <c r="AA31" s="38"/>
+      <c r="AA31" s="9"/>
       <c r="AB31" s="38"/>
-      <c r="AC31" s="20"/>
-      <c r="AD31" s="29" t="s">
+      <c r="AC31" s="38"/>
+      <c r="AD31" s="20"/>
+      <c r="AE31" s="29" t="s">
         <v>426</v>
       </c>
-      <c r="AE31" s="29" t="s">
+      <c r="AF31" s="29" t="s">
         <v>423</v>
       </c>
-      <c r="AF31" s="29" t="s">
+      <c r="AG31" s="29" t="s">
         <v>425</v>
       </c>
-      <c r="AG31" s="35">
+      <c r="AH31" s="35">
         <v>9</v>
       </c>
-      <c r="AH31" s="35" t="s">
+      <c r="AI31" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="AI31" s="35" t="s">
+      <c r="AJ31" s="35" t="s">
         <v>418</v>
       </c>
-      <c r="AJ31" s="35">
+      <c r="AK31" s="35">
         <v>2022</v>
       </c>
-      <c r="AK31" s="35" t="s">
+      <c r="AL31" s="35" t="s">
         <v>372</v>
       </c>
-      <c r="AL31" s="35"/>
-      <c r="AM31" s="35"/>
-      <c r="AN31" s="35"/>
+      <c r="AM31" s="49"/>
+      <c r="AN31" s="49"/>
       <c r="AO31" s="35"/>
       <c r="AP31" s="35"/>
       <c r="AQ31" s="35"/>
       <c r="AR31" s="35"/>
       <c r="AS31" s="35"/>
-      <c r="AT31" s="20"/>
+      <c r="AT31" s="35"/>
       <c r="AU31" s="20"/>
       <c r="AV31" s="20"/>
       <c r="AW31" s="20"/>
       <c r="AX31" s="20"/>
-      <c r="AY31" s="20"/>
-      <c r="AZ31" s="20"/>
+      <c r="AY31" s="27"/>
+      <c r="AZ31" s="27"/>
       <c r="BA31" s="20"/>
-    </row>
-    <row r="32" spans="1:53" ht="15.75">
+      <c r="BB31" s="20"/>
+    </row>
+    <row r="32" spans="1:54" ht="15.75">
       <c r="A32" s="20" t="s">
         <v>316</v>
       </c>
@@ -7883,22 +7924,22 @@
       <c r="N32" s="34"/>
       <c r="O32" s="34"/>
       <c r="P32" s="34"/>
-      <c r="Q32" s="9"/>
+      <c r="Q32" s="34"/>
       <c r="R32" s="9"/>
-      <c r="S32" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T32" s="9"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U32" s="9"/>
       <c r="V32" s="9"/>
       <c r="W32" s="9"/>
       <c r="X32" s="9"/>
       <c r="Y32" s="9"/>
       <c r="Z32" s="9"/>
-      <c r="AA32" s="38"/>
+      <c r="AA32" s="9"/>
       <c r="AB32" s="38"/>
-      <c r="AC32" s="20"/>
-      <c r="AD32" s="35"/>
+      <c r="AC32" s="38"/>
+      <c r="AD32" s="20"/>
       <c r="AE32" s="35"/>
       <c r="AF32" s="35"/>
       <c r="AG32" s="35"/>
@@ -7906,40 +7947,41 @@
       <c r="AI32" s="35"/>
       <c r="AJ32" s="35"/>
       <c r="AK32" s="35"/>
-      <c r="AL32" s="29" t="s">
+      <c r="AL32" s="35"/>
+      <c r="AM32" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="AM32" s="29" t="s">
+      <c r="AN32" s="34" t="s">
         <v>416</v>
       </c>
-      <c r="AN32" s="29" t="s">
+      <c r="AO32" s="29" t="s">
         <v>417</v>
       </c>
-      <c r="AO32" s="35">
+      <c r="AP32" s="35">
         <v>6</v>
       </c>
-      <c r="AP32" s="35" t="s">
+      <c r="AQ32" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="AQ32" s="35" t="s">
+      <c r="AR32" s="35" t="s">
         <v>418</v>
       </c>
-      <c r="AR32" s="35">
+      <c r="AS32" s="35">
         <v>2022</v>
       </c>
-      <c r="AS32" s="35" t="s">
+      <c r="AT32" s="35" t="s">
         <v>372</v>
       </c>
-      <c r="AT32" s="20"/>
       <c r="AU32" s="20"/>
       <c r="AV32" s="20"/>
       <c r="AW32" s="20"/>
       <c r="AX32" s="20"/>
-      <c r="AY32" s="20"/>
-      <c r="AZ32" s="20"/>
+      <c r="AY32" s="27"/>
+      <c r="AZ32" s="27"/>
       <c r="BA32" s="20"/>
-    </row>
-    <row r="33" spans="1:53" ht="15.75">
+      <c r="BB32" s="20"/>
+    </row>
+    <row r="33" spans="1:54" ht="15.75">
       <c r="A33" s="20" t="s">
         <v>318</v>
       </c>
@@ -7960,27 +8002,27 @@
       <c r="N33" s="34"/>
       <c r="O33" s="34"/>
       <c r="P33" s="34"/>
-      <c r="Q33" s="9"/>
+      <c r="Q33" s="34"/>
       <c r="R33" s="9"/>
-      <c r="S33" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T33" s="9"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U33" s="9"/>
       <c r="V33" s="9"/>
       <c r="W33" s="9"/>
       <c r="X33" s="9"/>
       <c r="Y33" s="9"/>
       <c r="Z33" s="9"/>
-      <c r="AA33" s="38" t="s">
+      <c r="AA33" s="9"/>
+      <c r="AB33" s="38" t="s">
         <v>438</v>
       </c>
-      <c r="AB33" s="38"/>
-      <c r="AC33" s="20"/>
-      <c r="AD33" s="29" t="s">
+      <c r="AC33" s="38"/>
+      <c r="AD33" s="20"/>
+      <c r="AE33" s="29" t="s">
         <v>360</v>
       </c>
-      <c r="AE33" s="35"/>
       <c r="AF33" s="35"/>
       <c r="AG33" s="35"/>
       <c r="AH33" s="35"/>
@@ -7988,23 +8030,24 @@
       <c r="AJ33" s="35"/>
       <c r="AK33" s="35"/>
       <c r="AL33" s="35"/>
-      <c r="AM33" s="35"/>
-      <c r="AN33" s="35"/>
+      <c r="AM33" s="49"/>
+      <c r="AN33" s="49"/>
       <c r="AO33" s="35"/>
       <c r="AP33" s="35"/>
       <c r="AQ33" s="35"/>
       <c r="AR33" s="35"/>
       <c r="AS33" s="35"/>
-      <c r="AT33" s="20"/>
+      <c r="AT33" s="35"/>
       <c r="AU33" s="20"/>
       <c r="AV33" s="20"/>
       <c r="AW33" s="20"/>
       <c r="AX33" s="20"/>
-      <c r="AY33" s="20"/>
-      <c r="AZ33" s="20"/>
+      <c r="AY33" s="27"/>
+      <c r="AZ33" s="27"/>
       <c r="BA33" s="20"/>
-    </row>
-    <row r="34" spans="1:53" ht="15.75">
+      <c r="BB33" s="20"/>
+    </row>
+    <row r="34" spans="1:54" ht="15.75">
       <c r="A34" s="20" t="s">
         <v>320</v>
       </c>
@@ -8025,27 +8068,27 @@
       <c r="N34" s="34"/>
       <c r="O34" s="34"/>
       <c r="P34" s="34"/>
-      <c r="Q34" s="9"/>
+      <c r="Q34" s="34"/>
       <c r="R34" s="9"/>
-      <c r="S34" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T34" s="9"/>
+      <c r="S34" s="9"/>
+      <c r="T34" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U34" s="9"/>
       <c r="V34" s="9"/>
       <c r="W34" s="9"/>
       <c r="X34" s="9"/>
       <c r="Y34" s="9"/>
       <c r="Z34" s="9"/>
-      <c r="AA34" s="38" t="s">
+      <c r="AA34" s="9"/>
+      <c r="AB34" s="38" t="s">
         <v>439</v>
       </c>
-      <c r="AB34" s="38"/>
-      <c r="AC34" s="20"/>
-      <c r="AD34" s="29" t="s">
+      <c r="AC34" s="38"/>
+      <c r="AD34" s="20"/>
+      <c r="AE34" s="29" t="s">
         <v>360</v>
       </c>
-      <c r="AE34" s="35"/>
       <c r="AF34" s="35"/>
       <c r="AG34" s="35"/>
       <c r="AH34" s="35"/>
@@ -8053,23 +8096,24 @@
       <c r="AJ34" s="35"/>
       <c r="AK34" s="35"/>
       <c r="AL34" s="35"/>
-      <c r="AM34" s="35"/>
-      <c r="AN34" s="35"/>
+      <c r="AM34" s="49"/>
+      <c r="AN34" s="49"/>
       <c r="AO34" s="35"/>
       <c r="AP34" s="35"/>
       <c r="AQ34" s="35"/>
       <c r="AR34" s="35"/>
       <c r="AS34" s="35"/>
-      <c r="AT34" s="20"/>
+      <c r="AT34" s="35"/>
       <c r="AU34" s="20"/>
       <c r="AV34" s="20"/>
       <c r="AW34" s="20"/>
       <c r="AX34" s="20"/>
-      <c r="AY34" s="20"/>
-      <c r="AZ34" s="20"/>
+      <c r="AY34" s="27"/>
+      <c r="AZ34" s="27"/>
       <c r="BA34" s="20"/>
-    </row>
-    <row r="35" spans="1:53" ht="15.75">
+      <c r="BB34" s="20"/>
+    </row>
+    <row r="35" spans="1:54" ht="15.75">
       <c r="A35" s="20" t="s">
         <v>321</v>
       </c>
@@ -8090,22 +8134,22 @@
       <c r="N35" s="34"/>
       <c r="O35" s="34"/>
       <c r="P35" s="34"/>
-      <c r="Q35" s="9"/>
+      <c r="Q35" s="34"/>
       <c r="R35" s="9"/>
-      <c r="S35" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T35" s="9"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U35" s="9"/>
       <c r="V35" s="9"/>
       <c r="W35" s="9"/>
       <c r="X35" s="9"/>
       <c r="Y35" s="9"/>
       <c r="Z35" s="9"/>
-      <c r="AA35" s="38"/>
+      <c r="AA35" s="9"/>
       <c r="AB35" s="38"/>
-      <c r="AC35" s="20"/>
-      <c r="AD35" s="35"/>
+      <c r="AC35" s="38"/>
+      <c r="AD35" s="20"/>
       <c r="AE35" s="35"/>
       <c r="AF35" s="35"/>
       <c r="AG35" s="35"/>
@@ -8114,23 +8158,24 @@
       <c r="AJ35" s="35"/>
       <c r="AK35" s="35"/>
       <c r="AL35" s="35"/>
-      <c r="AM35" s="35"/>
-      <c r="AN35" s="35"/>
+      <c r="AM35" s="49"/>
+      <c r="AN35" s="49"/>
       <c r="AO35" s="35"/>
       <c r="AP35" s="35"/>
       <c r="AQ35" s="35"/>
       <c r="AR35" s="35"/>
       <c r="AS35" s="35"/>
-      <c r="AT35" s="20"/>
+      <c r="AT35" s="35"/>
       <c r="AU35" s="20"/>
       <c r="AV35" s="20"/>
       <c r="AW35" s="20"/>
       <c r="AX35" s="20"/>
-      <c r="AY35" s="20"/>
-      <c r="AZ35" s="20"/>
+      <c r="AY35" s="27"/>
+      <c r="AZ35" s="27"/>
       <c r="BA35" s="20"/>
-    </row>
-    <row r="36" spans="1:53" ht="15.75">
+      <c r="BB35" s="20"/>
+    </row>
+    <row r="36" spans="1:54" ht="15.75">
       <c r="A36" s="20" t="s">
         <v>324</v>
       </c>
@@ -8151,22 +8196,22 @@
       <c r="N36" s="34"/>
       <c r="O36" s="34"/>
       <c r="P36" s="34"/>
-      <c r="Q36" s="9"/>
+      <c r="Q36" s="34"/>
       <c r="R36" s="9"/>
-      <c r="S36" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T36" s="9"/>
+      <c r="S36" s="9"/>
+      <c r="T36" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U36" s="9"/>
       <c r="V36" s="9"/>
       <c r="W36" s="9"/>
       <c r="X36" s="9"/>
       <c r="Y36" s="9"/>
       <c r="Z36" s="9"/>
-      <c r="AA36" s="38"/>
+      <c r="AA36" s="9"/>
       <c r="AB36" s="38"/>
-      <c r="AC36" s="20"/>
-      <c r="AD36" s="35"/>
+      <c r="AC36" s="38"/>
+      <c r="AD36" s="20"/>
       <c r="AE36" s="35"/>
       <c r="AF36" s="35"/>
       <c r="AG36" s="35"/>
@@ -8175,16 +8220,14 @@
       <c r="AJ36" s="35"/>
       <c r="AK36" s="35"/>
       <c r="AL36" s="35"/>
-      <c r="AM36" s="35"/>
-      <c r="AN36" s="35"/>
+      <c r="AM36" s="49"/>
+      <c r="AN36" s="49"/>
       <c r="AO36" s="35"/>
       <c r="AP36" s="35"/>
       <c r="AQ36" s="35"/>
       <c r="AR36" s="35"/>
       <c r="AS36" s="35"/>
-      <c r="AT36" s="20" t="s">
-        <v>450</v>
-      </c>
+      <c r="AT36" s="35"/>
       <c r="AU36" s="20" t="s">
         <v>450</v>
       </c>
@@ -8192,22 +8235,25 @@
         <v>450</v>
       </c>
       <c r="AW36" s="20" t="s">
+        <v>450</v>
+      </c>
+      <c r="AX36" s="20" t="s">
         <v>451</v>
       </c>
-      <c r="AX36" s="20" t="s">
+      <c r="AY36" s="27" t="s">
         <v>449</v>
       </c>
-      <c r="AY36" s="20" t="s">
+      <c r="AZ36" s="27" t="s">
         <v>448</v>
       </c>
-      <c r="AZ36" s="20">
+      <c r="BA36" s="20">
         <v>10</v>
       </c>
-      <c r="BA36" s="20">
+      <c r="BB36" s="20">
         <v>1001</v>
       </c>
     </row>
-    <row r="37" spans="1:53" ht="15.75">
+    <row r="37" spans="1:54" ht="15.75">
       <c r="A37" s="20" t="s">
         <v>326</v>
       </c>
@@ -8228,22 +8274,22 @@
       <c r="N37" s="34"/>
       <c r="O37" s="34"/>
       <c r="P37" s="34"/>
-      <c r="Q37" s="9"/>
+      <c r="Q37" s="34"/>
       <c r="R37" s="9"/>
-      <c r="S37" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T37" s="9"/>
+      <c r="S37" s="9"/>
+      <c r="T37" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U37" s="9"/>
       <c r="V37" s="9"/>
       <c r="W37" s="9"/>
       <c r="X37" s="9"/>
       <c r="Y37" s="9"/>
       <c r="Z37" s="9"/>
-      <c r="AA37" s="38"/>
+      <c r="AA37" s="9"/>
       <c r="AB37" s="38"/>
-      <c r="AC37" s="20"/>
-      <c r="AD37" s="35"/>
+      <c r="AC37" s="38"/>
+      <c r="AD37" s="20"/>
       <c r="AE37" s="35"/>
       <c r="AF37" s="35"/>
       <c r="AG37" s="35"/>
@@ -8252,23 +8298,24 @@
       <c r="AJ37" s="35"/>
       <c r="AK37" s="35"/>
       <c r="AL37" s="35"/>
-      <c r="AM37" s="35"/>
-      <c r="AN37" s="35"/>
+      <c r="AM37" s="49"/>
+      <c r="AN37" s="49"/>
       <c r="AO37" s="35"/>
       <c r="AP37" s="35"/>
       <c r="AQ37" s="35"/>
       <c r="AR37" s="35"/>
       <c r="AS37" s="35"/>
-      <c r="AT37" s="20"/>
+      <c r="AT37" s="35"/>
       <c r="AU37" s="20"/>
       <c r="AV37" s="20"/>
       <c r="AW37" s="20"/>
       <c r="AX37" s="20"/>
-      <c r="AY37" s="20"/>
-      <c r="AZ37" s="20"/>
+      <c r="AY37" s="27"/>
+      <c r="AZ37" s="27"/>
       <c r="BA37" s="20"/>
-    </row>
-    <row r="38" spans="1:53" ht="15.75">
+      <c r="BB37" s="20"/>
+    </row>
+    <row r="38" spans="1:54" ht="15.75">
       <c r="A38" s="20" t="s">
         <v>328</v>
       </c>
@@ -8289,22 +8336,22 @@
       <c r="N38" s="34"/>
       <c r="O38" s="34"/>
       <c r="P38" s="34"/>
-      <c r="Q38" s="9"/>
+      <c r="Q38" s="34"/>
       <c r="R38" s="9"/>
-      <c r="S38" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T38" s="9"/>
+      <c r="S38" s="9"/>
+      <c r="T38" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U38" s="9"/>
       <c r="V38" s="9"/>
       <c r="W38" s="9"/>
       <c r="X38" s="9"/>
       <c r="Y38" s="9"/>
       <c r="Z38" s="9"/>
-      <c r="AA38" s="38"/>
+      <c r="AA38" s="9"/>
       <c r="AB38" s="38"/>
-      <c r="AC38" s="20"/>
-      <c r="AD38" s="35"/>
+      <c r="AC38" s="38"/>
+      <c r="AD38" s="20"/>
       <c r="AE38" s="35"/>
       <c r="AF38" s="35"/>
       <c r="AG38" s="35"/>
@@ -8313,23 +8360,24 @@
       <c r="AJ38" s="35"/>
       <c r="AK38" s="35"/>
       <c r="AL38" s="35"/>
-      <c r="AM38" s="35"/>
-      <c r="AN38" s="35"/>
+      <c r="AM38" s="49"/>
+      <c r="AN38" s="49"/>
       <c r="AO38" s="35"/>
       <c r="AP38" s="35"/>
       <c r="AQ38" s="35"/>
       <c r="AR38" s="35"/>
       <c r="AS38" s="35"/>
-      <c r="AT38" s="20"/>
+      <c r="AT38" s="35"/>
       <c r="AU38" s="20"/>
       <c r="AV38" s="20"/>
       <c r="AW38" s="20"/>
       <c r="AX38" s="20"/>
-      <c r="AY38" s="20"/>
-      <c r="AZ38" s="20"/>
+      <c r="AY38" s="27"/>
+      <c r="AZ38" s="27"/>
       <c r="BA38" s="20"/>
-    </row>
-    <row r="39" spans="1:53" ht="15.75">
+      <c r="BB38" s="20"/>
+    </row>
+    <row r="39" spans="1:54" ht="15.75">
       <c r="A39" s="20" t="s">
         <v>329</v>
       </c>
@@ -8350,22 +8398,22 @@
       <c r="N39" s="34"/>
       <c r="O39" s="34"/>
       <c r="P39" s="34"/>
-      <c r="Q39" s="9"/>
+      <c r="Q39" s="34"/>
       <c r="R39" s="9"/>
-      <c r="S39" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T39" s="9"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U39" s="9"/>
       <c r="V39" s="9"/>
       <c r="W39" s="9"/>
       <c r="X39" s="9"/>
       <c r="Y39" s="9"/>
       <c r="Z39" s="9"/>
-      <c r="AA39" s="38"/>
+      <c r="AA39" s="9"/>
       <c r="AB39" s="38"/>
-      <c r="AC39" s="20"/>
-      <c r="AD39" s="35"/>
+      <c r="AC39" s="38"/>
+      <c r="AD39" s="20"/>
       <c r="AE39" s="35"/>
       <c r="AF39" s="35"/>
       <c r="AG39" s="35"/>
@@ -8374,23 +8422,24 @@
       <c r="AJ39" s="35"/>
       <c r="AK39" s="35"/>
       <c r="AL39" s="35"/>
-      <c r="AM39" s="35"/>
-      <c r="AN39" s="35"/>
+      <c r="AM39" s="49"/>
+      <c r="AN39" s="49"/>
       <c r="AO39" s="35"/>
       <c r="AP39" s="35"/>
       <c r="AQ39" s="35"/>
       <c r="AR39" s="35"/>
       <c r="AS39" s="35"/>
-      <c r="AT39" s="20"/>
+      <c r="AT39" s="35"/>
       <c r="AU39" s="20"/>
       <c r="AV39" s="20"/>
       <c r="AW39" s="20"/>
       <c r="AX39" s="20"/>
-      <c r="AY39" s="20"/>
-      <c r="AZ39" s="20"/>
+      <c r="AY39" s="27"/>
+      <c r="AZ39" s="27"/>
       <c r="BA39" s="20"/>
-    </row>
-    <row r="40" spans="1:53" ht="15.75">
+      <c r="BB39" s="20"/>
+    </row>
+    <row r="40" spans="1:54" ht="15.75">
       <c r="A40" s="20" t="s">
         <v>332</v>
       </c>
@@ -8411,22 +8460,22 @@
       <c r="N40" s="34"/>
       <c r="O40" s="34"/>
       <c r="P40" s="34"/>
-      <c r="Q40" s="9"/>
+      <c r="Q40" s="34"/>
       <c r="R40" s="9"/>
-      <c r="S40" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T40" s="9"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U40" s="9"/>
       <c r="V40" s="9"/>
       <c r="W40" s="9"/>
       <c r="X40" s="9"/>
       <c r="Y40" s="9"/>
       <c r="Z40" s="9"/>
-      <c r="AA40" s="38"/>
+      <c r="AA40" s="9"/>
       <c r="AB40" s="38"/>
-      <c r="AC40" s="20"/>
-      <c r="AD40" s="35"/>
+      <c r="AC40" s="38"/>
+      <c r="AD40" s="20"/>
       <c r="AE40" s="35"/>
       <c r="AF40" s="35"/>
       <c r="AG40" s="35"/>
@@ -8435,23 +8484,24 @@
       <c r="AJ40" s="35"/>
       <c r="AK40" s="35"/>
       <c r="AL40" s="35"/>
-      <c r="AM40" s="35"/>
-      <c r="AN40" s="35"/>
+      <c r="AM40" s="49"/>
+      <c r="AN40" s="49"/>
       <c r="AO40" s="35"/>
       <c r="AP40" s="35"/>
       <c r="AQ40" s="35"/>
       <c r="AR40" s="35"/>
       <c r="AS40" s="35"/>
-      <c r="AT40" s="20"/>
+      <c r="AT40" s="35"/>
       <c r="AU40" s="20"/>
       <c r="AV40" s="20"/>
       <c r="AW40" s="20"/>
       <c r="AX40" s="20"/>
-      <c r="AY40" s="20"/>
-      <c r="AZ40" s="20"/>
+      <c r="AY40" s="27"/>
+      <c r="AZ40" s="27"/>
       <c r="BA40" s="20"/>
-    </row>
-    <row r="41" spans="1:53" ht="15.75">
+      <c r="BB40" s="20"/>
+    </row>
+    <row r="41" spans="1:54" ht="15.75">
       <c r="A41" s="20" t="s">
         <v>333</v>
       </c>
@@ -8472,22 +8522,22 @@
       <c r="N41" s="34"/>
       <c r="O41" s="34"/>
       <c r="P41" s="34"/>
-      <c r="Q41" s="9"/>
+      <c r="Q41" s="34"/>
       <c r="R41" s="9"/>
-      <c r="S41" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T41" s="9"/>
+      <c r="S41" s="9"/>
+      <c r="T41" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U41" s="9"/>
       <c r="V41" s="9"/>
       <c r="W41" s="9"/>
       <c r="X41" s="9"/>
       <c r="Y41" s="9"/>
       <c r="Z41" s="9"/>
-      <c r="AA41" s="38"/>
+      <c r="AA41" s="9"/>
       <c r="AB41" s="38"/>
-      <c r="AC41" s="20"/>
-      <c r="AD41" s="35"/>
+      <c r="AC41" s="38"/>
+      <c r="AD41" s="20"/>
       <c r="AE41" s="35"/>
       <c r="AF41" s="35"/>
       <c r="AG41" s="35"/>
@@ -8496,23 +8546,24 @@
       <c r="AJ41" s="35"/>
       <c r="AK41" s="35"/>
       <c r="AL41" s="35"/>
-      <c r="AM41" s="35"/>
-      <c r="AN41" s="35"/>
+      <c r="AM41" s="49"/>
+      <c r="AN41" s="49"/>
       <c r="AO41" s="35"/>
       <c r="AP41" s="35"/>
       <c r="AQ41" s="35"/>
       <c r="AR41" s="35"/>
       <c r="AS41" s="35"/>
-      <c r="AT41" s="20"/>
+      <c r="AT41" s="35"/>
       <c r="AU41" s="20"/>
       <c r="AV41" s="20"/>
       <c r="AW41" s="20"/>
       <c r="AX41" s="20"/>
-      <c r="AY41" s="20"/>
-      <c r="AZ41" s="20"/>
+      <c r="AY41" s="27"/>
+      <c r="AZ41" s="27"/>
       <c r="BA41" s="20"/>
-    </row>
-    <row r="42" spans="1:53" ht="15.75">
+      <c r="BB41" s="20"/>
+    </row>
+    <row r="42" spans="1:54" ht="15.75">
       <c r="A42" s="20" t="s">
         <v>336</v>
       </c>
@@ -8532,23 +8583,29 @@
       <c r="M42" s="34"/>
       <c r="N42" s="34"/>
       <c r="O42" s="34"/>
-      <c r="P42" s="34"/>
-      <c r="Q42" s="9"/>
-      <c r="R42" s="9"/>
-      <c r="S42" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T42" s="9"/>
+      <c r="P42" s="34" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q42" s="34" t="s">
+        <v>416</v>
+      </c>
+      <c r="R42" s="34" t="s">
+        <v>372</v>
+      </c>
+      <c r="S42" s="9"/>
+      <c r="T42" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U42" s="9"/>
       <c r="V42" s="9"/>
       <c r="W42" s="9"/>
       <c r="X42" s="9"/>
       <c r="Y42" s="9"/>
       <c r="Z42" s="9"/>
-      <c r="AA42" s="38"/>
+      <c r="AA42" s="9"/>
       <c r="AB42" s="38"/>
-      <c r="AC42" s="20"/>
-      <c r="AD42" s="35"/>
+      <c r="AC42" s="38"/>
+      <c r="AD42" s="20"/>
       <c r="AE42" s="35"/>
       <c r="AF42" s="35"/>
       <c r="AG42" s="35"/>
@@ -8557,23 +8614,24 @@
       <c r="AJ42" s="35"/>
       <c r="AK42" s="35"/>
       <c r="AL42" s="35"/>
-      <c r="AM42" s="35"/>
-      <c r="AN42" s="35"/>
+      <c r="AM42" s="49"/>
+      <c r="AN42" s="49"/>
       <c r="AO42" s="35"/>
       <c r="AP42" s="35"/>
       <c r="AQ42" s="35"/>
       <c r="AR42" s="35"/>
       <c r="AS42" s="35"/>
-      <c r="AT42" s="20"/>
+      <c r="AT42" s="35"/>
       <c r="AU42" s="20"/>
       <c r="AV42" s="20"/>
       <c r="AW42" s="20"/>
       <c r="AX42" s="20"/>
-      <c r="AY42" s="20"/>
-      <c r="AZ42" s="20"/>
+      <c r="AY42" s="27"/>
+      <c r="AZ42" s="27"/>
       <c r="BA42" s="20"/>
-    </row>
-    <row r="43" spans="1:53" ht="15.75">
+      <c r="BB42" s="20"/>
+    </row>
+    <row r="43" spans="1:54" ht="15.75">
       <c r="A43" s="20" t="s">
         <v>337</v>
       </c>
@@ -8593,23 +8651,29 @@
       <c r="M43" s="34"/>
       <c r="N43" s="34"/>
       <c r="O43" s="34"/>
-      <c r="P43" s="34"/>
-      <c r="Q43" s="9"/>
-      <c r="R43" s="9"/>
-      <c r="S43" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T43" s="9"/>
+      <c r="P43" s="34" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q43" s="34" t="s">
+        <v>416</v>
+      </c>
+      <c r="R43" s="34" t="s">
+        <v>372</v>
+      </c>
+      <c r="S43" s="9"/>
+      <c r="T43" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U43" s="9"/>
       <c r="V43" s="9"/>
       <c r="W43" s="9"/>
       <c r="X43" s="9"/>
       <c r="Y43" s="9"/>
       <c r="Z43" s="9"/>
-      <c r="AA43" s="38"/>
+      <c r="AA43" s="9"/>
       <c r="AB43" s="38"/>
-      <c r="AC43" s="20"/>
-      <c r="AD43" s="35"/>
+      <c r="AC43" s="38"/>
+      <c r="AD43" s="20"/>
       <c r="AE43" s="35"/>
       <c r="AF43" s="35"/>
       <c r="AG43" s="35"/>
@@ -8618,23 +8682,24 @@
       <c r="AJ43" s="35"/>
       <c r="AK43" s="35"/>
       <c r="AL43" s="35"/>
-      <c r="AM43" s="35"/>
-      <c r="AN43" s="35"/>
+      <c r="AM43" s="49"/>
+      <c r="AN43" s="49"/>
       <c r="AO43" s="35"/>
       <c r="AP43" s="35"/>
       <c r="AQ43" s="35"/>
       <c r="AR43" s="35"/>
       <c r="AS43" s="35"/>
-      <c r="AT43" s="20"/>
+      <c r="AT43" s="35"/>
       <c r="AU43" s="20"/>
       <c r="AV43" s="20"/>
       <c r="AW43" s="20"/>
       <c r="AX43" s="20"/>
-      <c r="AY43" s="20"/>
-      <c r="AZ43" s="20"/>
+      <c r="AY43" s="27"/>
+      <c r="AZ43" s="27"/>
       <c r="BA43" s="20"/>
-    </row>
-    <row r="44" spans="1:53" ht="15.75">
+      <c r="BB43" s="20"/>
+    </row>
+    <row r="44" spans="1:54" ht="15.75">
       <c r="A44" s="20" t="s">
         <v>340</v>
       </c>
@@ -8655,22 +8720,22 @@
       <c r="N44" s="34"/>
       <c r="O44" s="34"/>
       <c r="P44" s="34"/>
-      <c r="Q44" s="9"/>
+      <c r="Q44" s="34"/>
       <c r="R44" s="9"/>
-      <c r="S44" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T44" s="9"/>
+      <c r="S44" s="9"/>
+      <c r="T44" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U44" s="9"/>
       <c r="V44" s="9"/>
       <c r="W44" s="9"/>
       <c r="X44" s="9"/>
       <c r="Y44" s="9"/>
       <c r="Z44" s="9"/>
-      <c r="AA44" s="38"/>
+      <c r="AA44" s="9"/>
       <c r="AB44" s="38"/>
-      <c r="AC44" s="20"/>
-      <c r="AD44" s="35"/>
+      <c r="AC44" s="38"/>
+      <c r="AD44" s="20"/>
       <c r="AE44" s="35"/>
       <c r="AF44" s="35"/>
       <c r="AG44" s="35"/>
@@ -8679,23 +8744,24 @@
       <c r="AJ44" s="35"/>
       <c r="AK44" s="35"/>
       <c r="AL44" s="35"/>
-      <c r="AM44" s="35"/>
-      <c r="AN44" s="35"/>
+      <c r="AM44" s="49"/>
+      <c r="AN44" s="49"/>
       <c r="AO44" s="35"/>
       <c r="AP44" s="35"/>
       <c r="AQ44" s="35"/>
       <c r="AR44" s="35"/>
       <c r="AS44" s="35"/>
-      <c r="AT44" s="20"/>
+      <c r="AT44" s="35"/>
       <c r="AU44" s="20"/>
       <c r="AV44" s="20"/>
       <c r="AW44" s="20"/>
       <c r="AX44" s="20"/>
-      <c r="AY44" s="20"/>
-      <c r="AZ44" s="20"/>
+      <c r="AY44" s="27"/>
+      <c r="AZ44" s="27"/>
       <c r="BA44" s="20"/>
-    </row>
-    <row r="45" spans="1:53" ht="15.75">
+      <c r="BB44" s="20"/>
+    </row>
+    <row r="45" spans="1:54" ht="15.75">
       <c r="A45" s="20" t="s">
         <v>341</v>
       </c>
@@ -8715,23 +8781,29 @@
       <c r="M45" s="34"/>
       <c r="N45" s="34"/>
       <c r="O45" s="34"/>
-      <c r="P45" s="34"/>
-      <c r="Q45" s="9"/>
-      <c r="R45" s="9"/>
-      <c r="S45" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T45" s="9"/>
+      <c r="P45" s="34" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q45" s="34" t="s">
+        <v>416</v>
+      </c>
+      <c r="R45" s="34" t="s">
+        <v>372</v>
+      </c>
+      <c r="S45" s="9"/>
+      <c r="T45" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U45" s="9"/>
       <c r="V45" s="9"/>
       <c r="W45" s="9"/>
       <c r="X45" s="9"/>
       <c r="Y45" s="9"/>
       <c r="Z45" s="9"/>
-      <c r="AA45" s="38"/>
+      <c r="AA45" s="9"/>
       <c r="AB45" s="38"/>
-      <c r="AC45" s="20"/>
-      <c r="AD45" s="35"/>
+      <c r="AC45" s="38"/>
+      <c r="AD45" s="20"/>
       <c r="AE45" s="35"/>
       <c r="AF45" s="35"/>
       <c r="AG45" s="35"/>
@@ -8740,23 +8812,24 @@
       <c r="AJ45" s="35"/>
       <c r="AK45" s="35"/>
       <c r="AL45" s="35"/>
-      <c r="AM45" s="35"/>
-      <c r="AN45" s="35"/>
+      <c r="AM45" s="49"/>
+      <c r="AN45" s="49"/>
       <c r="AO45" s="35"/>
       <c r="AP45" s="35"/>
       <c r="AQ45" s="35"/>
       <c r="AR45" s="35"/>
       <c r="AS45" s="35"/>
-      <c r="AT45" s="20"/>
+      <c r="AT45" s="35"/>
       <c r="AU45" s="20"/>
       <c r="AV45" s="20"/>
       <c r="AW45" s="20"/>
       <c r="AX45" s="20"/>
-      <c r="AY45" s="20"/>
-      <c r="AZ45" s="20"/>
+      <c r="AY45" s="27"/>
+      <c r="AZ45" s="27"/>
       <c r="BA45" s="20"/>
-    </row>
-    <row r="46" spans="1:53" ht="15.75">
+      <c r="BB45" s="20"/>
+    </row>
+    <row r="46" spans="1:54" ht="15.75">
       <c r="A46" s="20" t="s">
         <v>344</v>
       </c>
@@ -8776,23 +8849,25 @@
       <c r="M46" s="34"/>
       <c r="N46" s="34"/>
       <c r="O46" s="34"/>
-      <c r="P46" s="34"/>
-      <c r="Q46" s="9"/>
+      <c r="P46" s="34" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q46" s="34"/>
       <c r="R46" s="9"/>
-      <c r="S46" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T46" s="9"/>
+      <c r="S46" s="9"/>
+      <c r="T46" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U46" s="9"/>
       <c r="V46" s="9"/>
       <c r="W46" s="9"/>
       <c r="X46" s="9"/>
       <c r="Y46" s="9"/>
       <c r="Z46" s="9"/>
-      <c r="AA46" s="38"/>
+      <c r="AA46" s="9"/>
       <c r="AB46" s="38"/>
-      <c r="AC46" s="20"/>
-      <c r="AD46" s="35"/>
+      <c r="AC46" s="38"/>
+      <c r="AD46" s="20"/>
       <c r="AE46" s="35"/>
       <c r="AF46" s="35"/>
       <c r="AG46" s="35"/>
@@ -8801,23 +8876,24 @@
       <c r="AJ46" s="35"/>
       <c r="AK46" s="35"/>
       <c r="AL46" s="35"/>
-      <c r="AM46" s="35"/>
-      <c r="AN46" s="35"/>
+      <c r="AM46" s="49"/>
+      <c r="AN46" s="49"/>
       <c r="AO46" s="35"/>
       <c r="AP46" s="35"/>
       <c r="AQ46" s="35"/>
       <c r="AR46" s="35"/>
       <c r="AS46" s="35"/>
-      <c r="AT46" s="20"/>
+      <c r="AT46" s="35"/>
       <c r="AU46" s="20"/>
       <c r="AV46" s="20"/>
       <c r="AW46" s="20"/>
       <c r="AX46" s="20"/>
-      <c r="AY46" s="20"/>
-      <c r="AZ46" s="20"/>
+      <c r="AY46" s="27"/>
+      <c r="AZ46" s="27"/>
       <c r="BA46" s="20"/>
-    </row>
-    <row r="47" spans="1:53" ht="15.75">
+      <c r="BB46" s="20"/>
+    </row>
+    <row r="47" spans="1:54" ht="15.75">
       <c r="A47" s="20" t="s">
         <v>345</v>
       </c>
@@ -8837,23 +8913,25 @@
       <c r="M47" s="34"/>
       <c r="N47" s="34"/>
       <c r="O47" s="34"/>
-      <c r="P47" s="34"/>
-      <c r="Q47" s="9"/>
+      <c r="P47" s="34" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q47" s="34"/>
       <c r="R47" s="9"/>
-      <c r="S47" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T47" s="9"/>
+      <c r="S47" s="9"/>
+      <c r="T47" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U47" s="9"/>
       <c r="V47" s="9"/>
       <c r="W47" s="9"/>
       <c r="X47" s="9"/>
       <c r="Y47" s="9"/>
       <c r="Z47" s="9"/>
-      <c r="AA47" s="38"/>
+      <c r="AA47" s="9"/>
       <c r="AB47" s="38"/>
-      <c r="AC47" s="20"/>
-      <c r="AD47" s="35"/>
+      <c r="AC47" s="38"/>
+      <c r="AD47" s="20"/>
       <c r="AE47" s="35"/>
       <c r="AF47" s="35"/>
       <c r="AG47" s="35"/>
@@ -8862,23 +8940,24 @@
       <c r="AJ47" s="35"/>
       <c r="AK47" s="35"/>
       <c r="AL47" s="35"/>
-      <c r="AM47" s="35"/>
-      <c r="AN47" s="35"/>
+      <c r="AM47" s="49"/>
+      <c r="AN47" s="49"/>
       <c r="AO47" s="35"/>
       <c r="AP47" s="35"/>
       <c r="AQ47" s="35"/>
       <c r="AR47" s="35"/>
       <c r="AS47" s="35"/>
-      <c r="AT47" s="20"/>
+      <c r="AT47" s="35"/>
       <c r="AU47" s="20"/>
       <c r="AV47" s="20"/>
       <c r="AW47" s="20"/>
       <c r="AX47" s="20"/>
-      <c r="AY47" s="20"/>
-      <c r="AZ47" s="20"/>
+      <c r="AY47" s="27"/>
+      <c r="AZ47" s="27"/>
       <c r="BA47" s="20"/>
-    </row>
-    <row r="48" spans="1:53" ht="15.75">
+      <c r="BB47" s="20"/>
+    </row>
+    <row r="48" spans="1:54" ht="15.75">
       <c r="A48" s="20" t="s">
         <v>346</v>
       </c>
@@ -8898,23 +8977,25 @@
       <c r="M48" s="34"/>
       <c r="N48" s="34"/>
       <c r="O48" s="34"/>
-      <c r="P48" s="34"/>
-      <c r="Q48" s="9"/>
+      <c r="P48" s="34" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q48" s="34"/>
       <c r="R48" s="9"/>
-      <c r="S48" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="T48" s="9"/>
+      <c r="S48" s="9"/>
+      <c r="T48" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="U48" s="9"/>
       <c r="V48" s="9"/>
       <c r="W48" s="9"/>
       <c r="X48" s="9"/>
       <c r="Y48" s="9"/>
       <c r="Z48" s="9"/>
-      <c r="AA48" s="38"/>
+      <c r="AA48" s="9"/>
       <c r="AB48" s="38"/>
-      <c r="AC48" s="20"/>
-      <c r="AD48" s="35"/>
+      <c r="AC48" s="38"/>
+      <c r="AD48" s="20"/>
       <c r="AE48" s="35"/>
       <c r="AF48" s="35"/>
       <c r="AG48" s="35"/>
@@ -8923,21 +9004,22 @@
       <c r="AJ48" s="35"/>
       <c r="AK48" s="35"/>
       <c r="AL48" s="35"/>
-      <c r="AM48" s="35"/>
-      <c r="AN48" s="35"/>
+      <c r="AM48" s="49"/>
+      <c r="AN48" s="49"/>
       <c r="AO48" s="35"/>
       <c r="AP48" s="35"/>
       <c r="AQ48" s="35"/>
       <c r="AR48" s="35"/>
       <c r="AS48" s="35"/>
-      <c r="AT48" s="20"/>
+      <c r="AT48" s="35"/>
       <c r="AU48" s="20"/>
       <c r="AV48" s="20"/>
       <c r="AW48" s="20"/>
       <c r="AX48" s="20"/>
-      <c r="AY48" s="20"/>
-      <c r="AZ48" s="20"/>
+      <c r="AY48" s="27"/>
+      <c r="AZ48" s="27"/>
       <c r="BA48" s="20"/>
+      <c r="BB48" s="20"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>